<commit_message>
Added more cerebro benchmark results
</commit_message>
<xml_diff>
--- a/Math/Lapack/SVD/svd_benchmarks.xlsx
+++ b/Math/Lapack/SVD/svd_benchmarks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="14">
   <si>
     <t>cluster</t>
   </si>
@@ -64,11 +64,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="GENERAL"/>
-    <numFmt numFmtId="167" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -98,6 +97,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -106,6 +106,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -117,14 +118,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -197,36 +198,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,10 +256,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:50"/>
+  <dimension ref="1:71"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I70" activeCellId="0" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -299,1571 +308,2243 @@
       <c r="AMJ1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="8" t="n">
         <f aca="false">1000*1000</f>
         <v>1000000</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="n">
+      <c r="C2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="n">
         <v>0.03576</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="8" t="n">
         <v>1.06</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="8" t="n">
         <v>0.1569</v>
       </c>
-      <c r="H2" s="7" t="n">
+      <c r="H2" s="9" t="n">
         <f aca="false">$F$2/(F2*$D2)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="7" t="n">
+      <c r="I2" s="9" t="n">
         <f aca="false">$G$2/(G2*$D2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="8" t="n">
         <f aca="false">1000*1000</f>
         <v>1000000</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="n">
+      <c r="C3" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="8" t="n">
         <v>0.008324</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="8" t="n">
         <v>0.6931</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="8" t="n">
         <v>0.0849</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H3" s="9" t="n">
         <f aca="false">$F$2/(F3*$D3)</f>
         <v>0.764680421295628</v>
       </c>
-      <c r="I3" s="7" t="n">
+      <c r="I3" s="9" t="n">
         <f aca="false">$G$2/(G3*$D3)</f>
         <v>0.924028268551237</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="8" t="n">
         <f aca="false">1000*1000</f>
         <v>1000000</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="n">
+      <c r="C4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="8" t="n">
         <v>0.008809</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="8" t="n">
         <v>0.5592</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="8" t="n">
         <v>0.04438</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="H4" s="9" t="n">
         <f aca="false">$F$2/(F4*$D4)</f>
         <v>0.473891273247496</v>
       </c>
-      <c r="I4" s="7" t="n">
+      <c r="I4" s="9" t="n">
         <f aca="false">$G$2/(G4*$D4)</f>
         <v>0.883844073907165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="8" t="n">
         <f aca="false">1000*1000</f>
         <v>1000000</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="n">
+      <c r="C5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="8" t="n">
         <v>0.008725</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="8" t="n">
         <v>0.5016</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="8" t="n">
         <v>0.02702</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="9" t="n">
         <f aca="false">$F$2/(F5*$D5)</f>
         <v>0.264154704944179</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="9" t="n">
         <f aca="false">$G$2/(G5*$D5)</f>
         <v>0.725851221317543</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="8" t="n">
         <f aca="false">1000*1000</f>
         <v>1000000</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="n">
+      <c r="C6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8" t="n">
         <v>0.00916</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="8" t="n">
         <v>0.4786</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="8" t="n">
         <v>0.02243</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="9" t="n">
         <f aca="false">$F$2/(F6*$D6)</f>
         <v>0.221479314667781</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="9" t="n">
         <f aca="false">$G$2/(G6*$D6)</f>
         <v>0.699509585376728</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="8" t="n">
         <f aca="false">1000*1000</f>
         <v>1000000</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="n">
+      <c r="C7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="8" t="n">
         <v>0.008274</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="8" t="n">
         <v>0.459</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="8" t="n">
         <v>0.0192</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="H7" s="9" t="n">
         <f aca="false">$F$2/(F7*$D7)</f>
         <v>0.144335511982571</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="9" t="n">
         <f aca="false">$G$2/(G7*$D7)</f>
         <v>0.5107421875</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="8" t="n">
         <f aca="false">1000*1000</f>
         <v>1000000</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="n">
+      <c r="C8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="8" t="n">
         <v>0.008693</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="8" t="n">
         <v>0.7924</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="8" t="n">
         <v>0.0268</v>
       </c>
-      <c r="H8" s="7" t="n">
+      <c r="H8" s="9" t="n">
         <f aca="false">$F$2/(F8*$D8)</f>
         <v>0.0668854114083796</v>
       </c>
-      <c r="I8" s="7" t="n">
+      <c r="I8" s="9" t="n">
         <f aca="false">$G$2/(G8*$D8)</f>
         <v>0.292723880597015</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="8" t="n">
         <f aca="false">2000*2000</f>
         <v>4000000</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="n">
+      <c r="C9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8" t="n">
         <v>0.3244</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="8" t="n">
         <v>7.662</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="8" t="n">
         <v>2.175</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H9" s="9" t="n">
         <f aca="false">$F$9/(F9*$D9)</f>
         <v>1</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I9" s="9" t="n">
         <f aca="false">$G$9/(G9*$D9)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="8" t="n">
         <f aca="false">2000*2000</f>
         <v>4000000</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="n">
+      <c r="C10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="8" t="n">
         <v>0.04366</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="8" t="n">
         <v>4.763</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="8" t="n">
         <v>1.582</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="H10" s="9" t="n">
         <f aca="false">$F$9/(F10*$D10)</f>
         <v>0.804325005248793</v>
       </c>
-      <c r="I10" s="7" t="n">
+      <c r="I10" s="9" t="n">
         <f aca="false">$G$9/(G10*$D10)</f>
         <v>0.687420986093552</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="8" t="n">
         <f aca="false">2000*2000</f>
         <v>4000000</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="n">
+      <c r="C11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="8" t="n">
         <v>0.04594</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="8" t="n">
         <v>3.027</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="8" t="n">
         <v>0.5269</v>
       </c>
-      <c r="H11" s="7" t="n">
+      <c r="H11" s="9" t="n">
         <f aca="false">$F$9/(F11*$D11)</f>
         <v>0.632804757185332</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="9" t="n">
         <f aca="false">$G$9/(G11*$D11)</f>
         <v>1.03197950275195</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="8" t="n">
         <f aca="false">2000*2000</f>
         <v>4000000</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="n">
+      <c r="C12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="8" t="n">
         <v>0.04602</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="8" t="n">
         <v>2.725</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="8" t="n">
         <v>1.007</v>
       </c>
-      <c r="H12" s="7" t="n">
+      <c r="H12" s="9" t="n">
         <f aca="false">$F$9/(F12*$D12)</f>
         <v>0.351467889908257</v>
       </c>
-      <c r="I12" s="7" t="n">
+      <c r="I12" s="9" t="n">
         <f aca="false">$G$9/(G12*$D12)</f>
         <v>0.269985104270109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="8" t="n">
         <f aca="false">2000*2000</f>
         <v>4000000</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2" t="n">
+      <c r="C13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" s="8" t="n">
         <v>0.0461</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="8" t="n">
         <v>2.324</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="8" t="n">
         <v>0.4895</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="9" t="n">
         <f aca="false">$F$9/(F13*$D13)</f>
         <v>0.329690189328744</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="9" t="n">
         <f aca="false">$G$9/(G13*$D13)</f>
         <v>0.444330949948927</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="8" t="n">
         <f aca="false">2000*2000</f>
         <v>4000000</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="n">
+      <c r="C14" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="8" t="n">
         <v>0.0463</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="8" t="n">
         <v>2.258</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="8" t="n">
         <v>0.4284</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="9" t="n">
         <f aca="false">$F$9/(F14*$D14)</f>
         <v>0.212079273693534</v>
       </c>
-      <c r="I14" s="7" t="n">
+      <c r="I14" s="9" t="n">
         <f aca="false">$G$9/(G14*$D14)</f>
         <v>0.317314425770308</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="8" t="n">
         <f aca="false">2000*2000</f>
         <v>4000000</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="n">
+      <c r="C15" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="8" t="n">
         <v>0.0456</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="8" t="n">
         <v>2.928</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="8" t="n">
         <v>0.9276</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="9" t="n">
         <f aca="false">$F$9/(F15*$D15)</f>
         <v>0.130840163934426</v>
       </c>
-      <c r="I15" s="7" t="n">
+      <c r="I15" s="9" t="n">
         <f aca="false">$G$9/(G15*$D15)</f>
         <v>0.117238033635188</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="8" t="n">
         <f aca="false">4000*4000</f>
         <v>16000000</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="n">
+      <c r="C16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="n">
         <v>2.917</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="8" t="n">
         <v>64.57</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="8" t="n">
         <v>9.804</v>
       </c>
-      <c r="H16" s="7" t="n">
+      <c r="H16" s="9" t="n">
         <f aca="false">$F$16/(F16*$D16)</f>
         <v>1</v>
       </c>
-      <c r="I16" s="7" t="n">
+      <c r="I16" s="9" t="n">
         <f aca="false">$G$16/(G16*$D16)</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="8" t="n">
         <f aca="false">4000*4000</f>
         <v>16000000</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="n">
+      <c r="C17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="8" t="n">
         <v>0.1944</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="8" t="n">
         <v>37.33</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="8" t="n">
         <v>5.75</v>
       </c>
-      <c r="H17" s="7" t="n">
+      <c r="H17" s="9" t="n">
         <f aca="false">$F$16/(F17*$D17)</f>
         <v>0.864854004821859</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I17" s="9" t="n">
         <f aca="false">$G$16/(G17*$D17)</f>
         <v>0.852521739130435</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="8" t="n">
         <f aca="false">4000*4000</f>
         <v>16000000</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="n">
+      <c r="C18" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="8" t="n">
         <v>0.1924</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="8" t="n">
         <v>22.32</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="8" t="n">
         <v>2.9</v>
       </c>
-      <c r="H18" s="7" t="n">
+      <c r="H18" s="9" t="n">
         <f aca="false">$F$16/(F18*$D18)</f>
         <v>0.723230286738351</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I18" s="9" t="n">
         <f aca="false">$G$16/(G18*$D18)</f>
         <v>0.845172413793103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="8" t="n">
         <f aca="false">4000*4000</f>
         <v>16000000</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="n">
+      <c r="C19" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="8" t="n">
         <v>0.1922</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="8" t="n">
         <v>17.5</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G19" s="8" t="n">
         <v>1.868</v>
       </c>
-      <c r="H19" s="7" t="n">
+      <c r="H19" s="9" t="n">
         <f aca="false">$F$16/(F19*$D19)</f>
         <v>0.461214285714286</v>
       </c>
-      <c r="I19" s="7" t="n">
+      <c r="I19" s="9" t="n">
         <f aca="false">$G$16/(G19*$D19)</f>
         <v>0.656049250535332</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="8" t="n">
         <f aca="false">4000*4000</f>
         <v>16000000</v>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="n">
+      <c r="C20" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" s="8" t="n">
         <v>0.1927</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="8" t="n">
         <v>15.77</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G20" s="8" t="n">
         <v>1.686</v>
       </c>
-      <c r="H20" s="7" t="n">
+      <c r="H20" s="9" t="n">
         <f aca="false">$F$16/(F20*$D20)</f>
         <v>0.409448319594166</v>
       </c>
-      <c r="I20" s="7" t="n">
+      <c r="I20" s="9" t="n">
         <f aca="false">$G$16/(G20*$D20)</f>
         <v>0.581494661921708</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="8" t="n">
         <f aca="false">4000*4000</f>
         <v>16000000</v>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="n">
+      <c r="C21" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="8" t="n">
         <v>0.1924</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="8" t="n">
         <v>14.83</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G21" s="8" t="n">
         <v>1.367</v>
       </c>
-      <c r="H21" s="7" t="n">
+      <c r="H21" s="9" t="n">
         <f aca="false">$F$16/(F21*$D21)</f>
         <v>0.272125758597438</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I21" s="9" t="n">
         <f aca="false">$G$16/(G21*$D21)</f>
         <v>0.448244330651061</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="8" t="n">
         <f aca="false">4000*4000</f>
         <v>16000000</v>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="n">
+      <c r="C22" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="8" t="n">
         <v>0.193</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="8" t="n">
         <v>14.58</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="8" t="n">
         <v>0.7935</v>
       </c>
-      <c r="H22" s="7" t="n">
+      <c r="H22" s="9" t="n">
         <f aca="false">$F$16/(F22*$D22)</f>
         <v>0.221433470507545</v>
       </c>
-      <c r="I22" s="7" t="n">
+      <c r="I22" s="9" t="n">
         <f aca="false">$G$16/(G22*$D22)</f>
         <v>0.617769376181475</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="2" t="n">
+      <c r="A23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2" t="n">
+      <c r="C23" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8" t="n">
         <v>2.943</v>
       </c>
-      <c r="F23" s="2" t="n">
+      <c r="F23" s="8" t="n">
         <v>628.6</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G23" s="8" t="n">
         <v>100.6</v>
       </c>
-      <c r="H23" s="7" t="n">
+      <c r="H23" s="9" t="n">
         <f aca="false">$F$23/(F23*$D23)</f>
         <v>1</v>
       </c>
-      <c r="I23" s="7" t="n">
+      <c r="I23" s="9" t="n">
         <f aca="false">$G$23/(G23*$D23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="2" t="n">
+      <c r="A24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="n">
+      <c r="C24" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E24" s="8" t="n">
         <v>4.396</v>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F24" s="8" t="n">
         <v>335.8</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G24" s="8" t="n">
         <v>51.24</v>
       </c>
-      <c r="H24" s="7" t="n">
+      <c r="H24" s="9" t="n">
         <f aca="false">$F$23/(F24*D24)</f>
         <v>0.935973793924955</v>
       </c>
-      <c r="I24" s="7" t="n">
+      <c r="I24" s="9" t="n">
         <f aca="false">$G$23/(G24*$D24)</f>
         <v>0.981654957064793</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="2" t="n">
+      <c r="A25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="n">
+      <c r="C25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="8" t="n">
         <v>1.533</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="8" t="n">
         <v>193.8</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="8" t="n">
         <v>26.15</v>
       </c>
-      <c r="H25" s="7" t="n">
+      <c r="H25" s="9" t="n">
         <f aca="false">$F$23/(F25*D25)</f>
         <v>0.810887512899897</v>
       </c>
-      <c r="I25" s="7" t="n">
+      <c r="I25" s="9" t="n">
         <f aca="false">$G$23/(G25*$D25)</f>
         <v>0.961759082217973</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="2" t="n">
+      <c r="A26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="n">
+      <c r="C26" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="8" t="n">
         <v>1.347</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F26" s="8" t="n">
         <v>140.3</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="8" t="n">
         <v>13.17</v>
       </c>
-      <c r="H26" s="7" t="n">
+      <c r="H26" s="9" t="n">
         <f aca="false">$F$23/(F26*D26)</f>
         <v>0.560049893086244</v>
       </c>
-      <c r="I26" s="7" t="n">
+      <c r="I26" s="9" t="n">
         <f aca="false">$G$23/(G26*$D26)</f>
         <v>0.954821564160972</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="2" t="n">
+      <c r="A27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E27" s="2" t="n">
+      <c r="C27" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E27" s="8" t="n">
         <v>2.898</v>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F27" s="8" t="n">
         <v>130</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="8" t="n">
         <v>11.02</v>
       </c>
-      <c r="H27" s="7" t="n">
+      <c r="H27" s="9" t="n">
         <f aca="false">$F$23/(F27*D27)</f>
         <v>0.483538461538462</v>
       </c>
-      <c r="I27" s="7" t="n">
+      <c r="I27" s="9" t="n">
         <f aca="false">$G$23/(G27*$D27)</f>
         <v>0.912885662431942</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="2" t="n">
+      <c r="A28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="n">
+      <c r="C28" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E28" s="2" t="n">
+      <c r="E28" s="8" t="n">
         <v>1.221</v>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F28" s="8" t="n">
         <v>191.1</v>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G28" s="8" t="n">
         <v>7.922</v>
       </c>
-      <c r="H28" s="7" t="n">
+      <c r="H28" s="9" t="n">
         <f aca="false">$F$23/(F28*D28)</f>
         <v>0.205586080586081</v>
       </c>
-      <c r="I28" s="7" t="n">
+      <c r="I28" s="9" t="n">
         <f aca="false">$G$23/(G28*$D28)</f>
         <v>0.793675839434486</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="2" t="n">
+      <c r="A29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="n">
+      <c r="C29" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="E29" s="2" t="n">
+      <c r="E29" s="8" t="n">
         <v>1.469</v>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F29" s="8" t="n">
         <v>238.4</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G29" s="8" t="n">
         <v>8.245</v>
       </c>
-      <c r="H29" s="7" t="n">
+      <c r="H29" s="9" t="n">
         <f aca="false">$F$23/(F29*D29)</f>
         <v>0.131837248322148</v>
       </c>
-      <c r="I29" s="7" t="n">
+      <c r="I29" s="9" t="n">
         <f aca="false">$G$23/(G29*$D29)</f>
         <v>0.610066707095209</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="B30" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="2" t="n">
+      <c r="C30" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8" t="n">
         <v>2.41</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F30" s="8" t="n">
         <v>526.8</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="8" t="n">
         <v>75.99</v>
       </c>
-      <c r="H30" s="7" t="n">
+      <c r="H30" s="9" t="n">
         <f aca="false">$F$30/(F30*D30)</f>
         <v>1</v>
       </c>
-      <c r="I30" s="7" t="n">
+      <c r="I30" s="9" t="n">
         <f aca="false">$G$30/(G30*$D30)</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C31" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="n">
+      <c r="C31" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E31" s="2" t="n">
+      <c r="E31" s="8" t="n">
         <v>0.7129</v>
       </c>
-      <c r="F31" s="2" t="n">
+      <c r="F31" s="8" t="n">
         <v>309.6</v>
       </c>
-      <c r="G31" s="2" t="n">
+      <c r="G31" s="8" t="n">
         <v>39.19</v>
       </c>
-      <c r="H31" s="7" t="n">
+      <c r="H31" s="9" t="n">
         <f aca="false">$F$30/(F31*D31)</f>
         <v>0.850775193798449</v>
       </c>
-      <c r="I31" s="7" t="n">
+      <c r="I31" s="9" t="n">
         <f aca="false">$G$30/(G31*$D31)</f>
         <v>0.969507527430467</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="2" t="n">
+      <c r="B32" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C32" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="n">
+      <c r="C32" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E32" s="2" t="n">
+      <c r="E32" s="8" t="n">
         <v>0.7184</v>
       </c>
-      <c r="F32" s="2" t="n">
+      <c r="F32" s="8" t="n">
         <v>174.7</v>
       </c>
-      <c r="G32" s="2" t="n">
+      <c r="G32" s="8" t="n">
         <v>20.84</v>
       </c>
-      <c r="H32" s="7" t="n">
+      <c r="H32" s="9" t="n">
         <f aca="false">$F$30/(F32*D32)</f>
         <v>0.753863766456783</v>
       </c>
-      <c r="I32" s="7" t="n">
+      <c r="I32" s="9" t="n">
         <f aca="false">$G$30/(G32*$D32)</f>
         <v>0.911588291746641</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="2" t="n">
+      <c r="B33" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C33" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2" t="n">
+      <c r="C33" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E33" s="2" t="n">
+      <c r="E33" s="8" t="n">
         <v>0.7147</v>
       </c>
-      <c r="F33" s="2" t="n">
+      <c r="F33" s="8" t="n">
         <v>127.3</v>
       </c>
-      <c r="G33" s="2" t="n">
+      <c r="G33" s="8" t="n">
         <v>11.2</v>
       </c>
-      <c r="H33" s="7" t="n">
+      <c r="H33" s="9" t="n">
         <f aca="false">$F$30/(F33*D33)</f>
         <v>0.517282010997643</v>
       </c>
-      <c r="I33" s="7" t="n">
+      <c r="I33" s="9" t="n">
         <f aca="false">$G$30/(G33*$D33)</f>
         <v>0.848102678571429</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="2" t="n">
+      <c r="B34" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C34" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E34" s="2" t="n">
+      <c r="C34" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E34" s="8" t="n">
         <v>0.7294</v>
       </c>
-      <c r="F34" s="2" t="n">
+      <c r="F34" s="8" t="n">
         <v>120.4</v>
       </c>
-      <c r="G34" s="2" t="n">
+      <c r="G34" s="8" t="n">
         <v>9.613</v>
       </c>
-      <c r="H34" s="7" t="n">
+      <c r="H34" s="9" t="n">
         <f aca="false">$F$30/(F34*D34)</f>
         <v>0.437541528239203</v>
       </c>
-      <c r="I34" s="7" t="n">
+      <c r="I34" s="9" t="n">
         <f aca="false">$G$30/(G34*$D34)</f>
         <v>0.790492042026423</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="2" t="n">
+      <c r="B35" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C35" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2" t="n">
+      <c r="C35" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E35" s="2" t="n">
+      <c r="E35" s="8" t="n">
         <v>0.7161</v>
       </c>
-      <c r="F35" s="2" t="n">
+      <c r="F35" s="8" t="n">
         <v>111.6</v>
       </c>
-      <c r="G35" s="2" t="n">
+      <c r="G35" s="8" t="n">
         <v>6.094</v>
       </c>
-      <c r="H35" s="7" t="n">
+      <c r="H35" s="9" t="n">
         <f aca="false">$F$30/(F35*D35)</f>
         <v>0.29502688172043</v>
       </c>
-      <c r="I35" s="7" t="n">
+      <c r="I35" s="9" t="n">
         <f aca="false">$G$30/(G35*$D35)</f>
         <v>0.779352641942895</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C36" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" s="2" t="n">
+      <c r="C36" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="E36" s="8" t="n">
         <v>0.715</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F36" s="8" t="n">
         <v>111.5</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G36" s="8" t="n">
         <v>5.383</v>
       </c>
-      <c r="H36" s="7" t="n">
+      <c r="H36" s="9" t="n">
         <f aca="false">$F$30/(F36*D36)</f>
         <v>0.236233183856502</v>
       </c>
-      <c r="I36" s="7" t="n">
+      <c r="I36" s="9" t="n">
         <f aca="false">$G$30/(G36*$D36)</f>
         <v>0.705833178524986</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="2" t="n">
+      <c r="A37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C37" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="2" t="n">
+      <c r="C37" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="8" t="n">
         <v>57.26</v>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="F37" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="G37" s="2" t="n">
+      <c r="G37" s="8" t="n">
         <v>802</v>
       </c>
-      <c r="H37" s="7" t="n">
+      <c r="H37" s="9" t="n">
         <f aca="false">$G$16/(G16*$D37)</f>
         <v>1</v>
       </c>
-      <c r="I37" s="7" t="n">
+      <c r="I37" s="9" t="n">
         <f aca="false">$H$16/(H16*$D37)</f>
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="2" t="n">
+      <c r="A38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C38" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" s="2" t="n">
+      <c r="C38" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E38" s="8" t="n">
         <v>58.62</v>
       </c>
-      <c r="F38" s="2" t="n">
+      <c r="F38" s="8" t="n">
         <v>2698</v>
       </c>
-      <c r="G38" s="2" t="n">
+      <c r="G38" s="8" t="n">
         <v>401.5</v>
       </c>
-      <c r="H38" s="7" t="n">
+      <c r="H38" s="9" t="n">
         <f aca="false">$G$16/(G17*$D38)</f>
         <v>0.528185009291761</v>
       </c>
-      <c r="I38" s="7" t="n">
+      <c r="I38" s="9" t="n">
         <f aca="false">$H$16/(H17*$D38)</f>
         <v>0.987068965517241</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="2" t="n">
+      <c r="A39" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C39" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D39" s="2" t="n">
+      <c r="C39" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E39" s="8" t="n">
         <v>57.26</v>
       </c>
-      <c r="F39" s="2" t="n">
+      <c r="F39" s="8" t="n">
         <v>1483</v>
       </c>
-      <c r="G39" s="2" t="n">
+      <c r="G39" s="8" t="n">
         <v>201.7</v>
       </c>
-      <c r="H39" s="7" t="n">
+      <c r="H39" s="9" t="n">
         <f aca="false">$G$16/(G18*$D39)</f>
         <v>0.264092504645881</v>
       </c>
-      <c r="I39" s="7" t="n">
+      <c r="I39" s="9" t="n">
         <f aca="false">$H$16/(H18*$D39)</f>
         <v>0.976010716025329</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="2" t="n">
+      <c r="A40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C40" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="n">
+      <c r="C40" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E40" s="2" t="n">
+      <c r="E40" s="8" t="n">
         <v>55.28</v>
       </c>
-      <c r="F40" s="2" t="n">
+      <c r="F40" s="8" t="n">
         <v>1044</v>
       </c>
-      <c r="G40" s="2" t="n">
+      <c r="G40" s="8" t="n">
         <v>101.5</v>
       </c>
-      <c r="H40" s="7" t="n">
+      <c r="H40" s="9" t="n">
         <f aca="false">$G$16/(G19*$D40)</f>
         <v>0.232039187227866</v>
       </c>
-      <c r="I40" s="7" t="n">
+      <c r="I40" s="9" t="n">
         <f aca="false">$H$16/(H19*$D40)</f>
         <v>0.958732057416268</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="2" t="n">
+      <c r="A41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C41" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E41" s="2" t="n">
+      <c r="C41" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E41" s="8" t="n">
         <v>55.96</v>
       </c>
-      <c r="F41" s="2" t="n">
+      <c r="F41" s="8" t="n">
         <v>967.5</v>
       </c>
-      <c r="G41" s="2" t="n">
+      <c r="G41" s="8" t="n">
         <v>81.76</v>
       </c>
-      <c r="H41" s="7" t="n">
+      <c r="H41" s="9" t="n">
         <f aca="false">$G$16/(G20*$D41)</f>
         <v>0.169403973509934</v>
       </c>
-      <c r="I41" s="7" t="n">
+      <c r="I41" s="9" t="n">
         <f aca="false">$H$16/(H20*$D41)</f>
         <v>0.953485605519867</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="2" t="n">
+      <c r="A42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C42" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2" t="n">
+      <c r="C42" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="8" t="n">
         <v>55.9</v>
       </c>
-      <c r="F42" s="2" t="n">
+      <c r="F42" s="8" t="n">
         <v>1539</v>
       </c>
-      <c r="G42" s="2" t="n">
+      <c r="G42" s="8" t="n">
         <v>52.99</v>
       </c>
-      <c r="H42" s="7" t="n">
+      <c r="H42" s="9" t="n">
         <f aca="false">$G$16/(G21*$D42)</f>
         <v>0.134915611814346</v>
       </c>
-      <c r="I42" s="7" t="n">
+      <c r="I42" s="9" t="n">
         <f aca="false">$H$16/(H21*$D42)</f>
         <v>0.811892220421394</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="2" t="n">
+      <c r="A43" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C43" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2" t="n">
+      <c r="C43" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="E43" s="2" t="n">
+      <c r="E43" s="8" t="n">
         <v>55.73</v>
       </c>
-      <c r="F43" s="2" t="n">
+      <c r="F43" s="8" t="n">
         <v>1948</v>
       </c>
-      <c r="G43" s="2" t="n">
+      <c r="G43" s="8" t="n">
         <v>48.79</v>
       </c>
-      <c r="H43" s="7" t="n">
+      <c r="H43" s="9" t="n">
         <f aca="false">$G$16/(G22*$D43)</f>
         <v>0.128028028028028</v>
       </c>
-      <c r="I43" s="7" t="n">
+      <c r="I43" s="9" t="n">
         <f aca="false">$H$16/(H22*$D43)</f>
         <v>0.775745257452575</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C44" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2" t="n">
+      <c r="C44" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="8" t="n">
         <v>39.86</v>
       </c>
-      <c r="F44" s="2" t="n">
+      <c r="F44" s="8" t="n">
         <v>4475</v>
       </c>
-      <c r="G44" s="2" t="n">
+      <c r="G44" s="8" t="n">
         <v>605.3</v>
       </c>
-      <c r="H44" s="7" t="n">
+      <c r="H44" s="9" t="n">
         <f aca="false">$F$44/(F44*$D44)</f>
         <v>1</v>
       </c>
-      <c r="I44" s="7" t="n">
+      <c r="I44" s="9" t="n">
         <f aca="false">$G$44/(G44*$D44)</f>
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="2" t="n">
+      <c r="B45" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C45" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="n">
+      <c r="C45" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E45" s="2" t="n">
+      <c r="E45" s="8" t="n">
         <v>38.86</v>
       </c>
-      <c r="F45" s="2" t="n">
+      <c r="F45" s="8" t="n">
         <v>2640</v>
       </c>
-      <c r="G45" s="2" t="n">
+      <c r="G45" s="8" t="n">
         <v>306.3</v>
       </c>
-      <c r="H45" s="7" t="n">
+      <c r="H45" s="9" t="n">
         <f aca="false">$F$44/(F45*$D45)</f>
         <v>0.847537878787879</v>
       </c>
-      <c r="I45" s="7" t="n">
+      <c r="I45" s="9" t="n">
         <f aca="false">$G$44/(G45*$D45)</f>
         <v>0.988083578191316</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="2" t="n">
+      <c r="B46" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C46" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D46" s="2" t="n">
+      <c r="C46" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E46" s="2" t="n">
+      <c r="E46" s="8" t="n">
         <v>36.48</v>
       </c>
-      <c r="F46" s="2" t="n">
+      <c r="F46" s="8" t="n">
         <v>1450</v>
       </c>
-      <c r="G46" s="2" t="n">
+      <c r="G46" s="8" t="n">
         <v>158.3</v>
       </c>
-      <c r="H46" s="7" t="n">
+      <c r="H46" s="9" t="n">
         <f aca="false">$F$44/(F46*$D46)</f>
         <v>0.771551724137931</v>
       </c>
-      <c r="I46" s="7" t="n">
+      <c r="I46" s="9" t="n">
         <f aca="false">$G$44/(G46*$D46)</f>
         <v>0.955938092229943</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="2" t="n">
+      <c r="B47" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C47" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2" t="n">
+      <c r="C47" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E47" s="2" t="n">
+      <c r="E47" s="8" t="n">
         <v>38.65</v>
       </c>
-      <c r="F47" s="2" t="n">
+      <c r="F47" s="8" t="n">
         <v>1012</v>
       </c>
-      <c r="G47" s="2" t="n">
+      <c r="G47" s="8" t="n">
         <v>84.39</v>
       </c>
-      <c r="H47" s="7" t="n">
+      <c r="H47" s="9" t="n">
         <f aca="false">$F$44/(F47*$D47)</f>
         <v>0.55274209486166</v>
       </c>
-      <c r="I47" s="7" t="n">
+      <c r="I47" s="9" t="n">
         <f aca="false">$G$44/(G47*$D47)</f>
         <v>0.896581348501007</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B48" s="2" t="n">
+      <c r="B48" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C48" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E48" s="2" t="n">
+      <c r="C48" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E48" s="8" t="n">
         <v>34.87</v>
       </c>
-      <c r="F48" s="2" t="n">
+      <c r="F48" s="8" t="n">
         <v>947.1</v>
       </c>
-      <c r="G48" s="2" t="n">
+      <c r="G48" s="8" t="n">
         <v>70.43</v>
       </c>
-      <c r="H48" s="7" t="n">
+      <c r="H48" s="9" t="n">
         <f aca="false">$F$44/(F48*$D48)</f>
         <v>0.472494984690107</v>
       </c>
-      <c r="I48" s="7" t="n">
+      <c r="I48" s="9" t="n">
         <f aca="false">$G$44/(G48*$D48)</f>
         <v>0.85943489990061</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="2" t="n">
+      <c r="B49" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C49" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2" t="n">
+      <c r="C49" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E49" s="2" t="n">
+      <c r="E49" s="8" t="n">
         <v>36.39</v>
       </c>
-      <c r="F49" s="2" t="n">
+      <c r="F49" s="8" t="n">
         <v>874.7</v>
       </c>
-      <c r="G49" s="2" t="n">
+      <c r="G49" s="8" t="n">
         <v>45.05</v>
       </c>
-      <c r="H49" s="7" t="n">
+      <c r="H49" s="9" t="n">
         <f aca="false">$F$44/(F49*$D49)</f>
         <v>0.319752486566823</v>
       </c>
-      <c r="I49" s="7" t="n">
+      <c r="I49" s="9" t="n">
         <f aca="false">$G$44/(G49*$D49)</f>
         <v>0.839761376248613</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="2" t="n">
+      <c r="B50" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C50" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="2" t="n">
+      <c r="C50" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="E50" s="2" t="n">
+      <c r="E50" s="8" t="n">
         <v>34.93</v>
       </c>
-      <c r="F50" s="2" t="n">
+      <c r="F50" s="8" t="n">
         <v>855.8</v>
       </c>
-      <c r="G50" s="2" t="n">
+      <c r="G50" s="8" t="n">
         <v>37.14</v>
       </c>
-      <c r="H50" s="7" t="n">
+      <c r="H50" s="9" t="n">
         <f aca="false">$F$44/(F50*$D50)</f>
         <v>0.261451273662071</v>
       </c>
-      <c r="I50" s="7" t="n">
+      <c r="I50" s="9" t="n">
         <f aca="false">$G$44/(G50*$D50)</f>
         <v>0.814889606892838</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="8" t="n">
+        <f aca="false">1000*1000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C51" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>6.594</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <v>1.537</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>0.2104</v>
+      </c>
+      <c r="H51" s="9" t="n">
+        <f aca="false">$F$51/(F51*$D51)</f>
+        <v>1</v>
+      </c>
+      <c r="I51" s="9" t="n">
+        <f aca="false">$G$51/(G51*$D51)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="8" t="n">
+        <f aca="false">1000*1000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C52" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>0.02268</v>
+      </c>
+      <c r="F52" s="2" t="n">
+        <v>0.8961</v>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>0.1089</v>
+      </c>
+      <c r="H52" s="9" t="n">
+        <f aca="false">$F$51/(F52*$D52)</f>
+        <v>0.857605177993527</v>
+      </c>
+      <c r="I52" s="9" t="n">
+        <f aca="false">$G$51/(G52*$D52)</f>
+        <v>0.966023875114784</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="8" t="n">
+        <f aca="false">1000*1000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C53" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>0.02567</v>
+      </c>
+      <c r="F53" s="2" t="n">
+        <v>0.6388</v>
+      </c>
+      <c r="G53" s="2" t="n">
+        <v>0.05813</v>
+      </c>
+      <c r="H53" s="9" t="n">
+        <f aca="false">$F$51/(F53*$D53)</f>
+        <v>0.601518472135254</v>
+      </c>
+      <c r="I53" s="9" t="n">
+        <f aca="false">$G$51/(G53*$D53)</f>
+        <v>0.90486839841734</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="8" t="n">
+        <f aca="false">1000*1000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C54" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="F54" s="2" t="n">
+        <v>0.6406</v>
+      </c>
+      <c r="G54" s="2" t="n">
+        <v>0.03669</v>
+      </c>
+      <c r="H54" s="9" t="n">
+        <f aca="false">$F$51/(F54*$D54)</f>
+        <v>0.299914142990946</v>
+      </c>
+      <c r="I54" s="9" t="n">
+        <f aca="false">$G$51/(G54*$D54)</f>
+        <v>0.716816571272826</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="8" t="n">
+        <f aca="false">1000*1000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C55" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>0.03054</v>
+      </c>
+      <c r="F55" s="2" t="n">
+        <v>0.6486</v>
+      </c>
+      <c r="G55" s="2" t="n">
+        <v>0.03051</v>
+      </c>
+      <c r="H55" s="9" t="n">
+        <f aca="false">$F$51/(F55*$D55)</f>
+        <v>0.236971939562134</v>
+      </c>
+      <c r="I55" s="9" t="n">
+        <f aca="false">$G$51/(G55*$D55)</f>
+        <v>0.689609963946247</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="8" t="n">
+        <f aca="false">1000*1000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C56" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>0.02427</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>0.7701</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>0.03541</v>
+      </c>
+      <c r="H56" s="9" t="n">
+        <f aca="false">$F$51/(F56*$D56)</f>
+        <v>0.124740293468381</v>
+      </c>
+      <c r="I56" s="9" t="n">
+        <f aca="false">$G$51/(G56*$D56)</f>
+        <v>0.371364021462864</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="8" t="n">
+        <f aca="false">1000*1000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C57" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>0.02996</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <v>0.6838</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>0.03274</v>
+      </c>
+      <c r="H57" s="9" t="n">
+        <f aca="false">$F$51/(F57*$D57)</f>
+        <v>0.112386662766891</v>
+      </c>
+      <c r="I57" s="9" t="n">
+        <f aca="false">$G$51/(G57*$D57)</f>
+        <v>0.321319486866219</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="8" t="n">
+        <f aca="false">2000*2000</f>
+        <v>4000000</v>
+      </c>
+      <c r="C58" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>2.066</v>
+      </c>
+      <c r="F58" s="2" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>2.135</v>
+      </c>
+      <c r="H58" s="9" t="n">
+        <f aca="false">$F$58/(F58*$D58)</f>
+        <v>1</v>
+      </c>
+      <c r="I58" s="9" t="n">
+        <f aca="false">$G$58/(G58*$D58)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="8" t="n">
+        <f aca="false">2000*2000</f>
+        <v>4000000</v>
+      </c>
+      <c r="C59" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="F59" s="2" t="n">
+        <v>5.737</v>
+      </c>
+      <c r="G59" s="2" t="n">
+        <v>1.219</v>
+      </c>
+      <c r="H59" s="9" t="n">
+        <f aca="false">$F$58/(F59*$D59)</f>
+        <v>0.897681715182151</v>
+      </c>
+      <c r="I59" s="9" t="n">
+        <f aca="false">$G$58/(G59*$D59)</f>
+        <v>0.87571780147662</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="8" t="n">
+        <f aca="false">2000*2000</f>
+        <v>4000000</v>
+      </c>
+      <c r="C60" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="F60" s="2" t="n">
+        <v>3.754</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>0.4578</v>
+      </c>
+      <c r="H60" s="9" t="n">
+        <f aca="false">$F$58/(F60*$D60)</f>
+        <v>0.685935002663825</v>
+      </c>
+      <c r="I60" s="9" t="n">
+        <f aca="false">$G$58/(G60*$D60)</f>
+        <v>1.16590214067278</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="8" t="n">
+        <f aca="false">2000*2000</f>
+        <v>4000000</v>
+      </c>
+      <c r="C61" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>0.1154</v>
+      </c>
+      <c r="F61" s="2" t="n">
+        <v>2.878</v>
+      </c>
+      <c r="G61" s="2" t="n">
+        <v>0.5059</v>
+      </c>
+      <c r="H61" s="9" t="n">
+        <f aca="false">$F$58/(F61*$D61)</f>
+        <v>0.447359277275886</v>
+      </c>
+      <c r="I61" s="9" t="n">
+        <f aca="false">$G$58/(G61*$D61)</f>
+        <v>0.527525202609211</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="8" t="n">
+        <f aca="false">2000*2000</f>
+        <v>4000000</v>
+      </c>
+      <c r="C62" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>0.1043</v>
+      </c>
+      <c r="F62" s="2" t="n">
+        <v>2.652</v>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>0.876</v>
+      </c>
+      <c r="H62" s="9" t="n">
+        <f aca="false">$F$58/(F62*$D62)</f>
+        <v>0.388386123680241</v>
+      </c>
+      <c r="I62" s="9" t="n">
+        <f aca="false">$G$58/(G62*$D62)</f>
+        <v>0.243721461187215</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="8" t="n">
+        <f aca="false">2000*2000</f>
+        <v>4000000</v>
+      </c>
+      <c r="C63" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>0.1112</v>
+      </c>
+      <c r="F63" s="2" t="n">
+        <v>3.414</v>
+      </c>
+      <c r="G63" s="2" t="n">
+        <v>0.3276</v>
+      </c>
+      <c r="H63" s="9" t="n">
+        <f aca="false">$F$58/(F63*$D63)</f>
+        <v>0.188561804335091</v>
+      </c>
+      <c r="I63" s="9" t="n">
+        <f aca="false">$G$58/(G63*$D63)</f>
+        <v>0.407318376068376</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="8" t="n">
+        <f aca="false">2000*2000</f>
+        <v>4000000</v>
+      </c>
+      <c r="C64" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>0.1057</v>
+      </c>
+      <c r="F64" s="2" t="n">
+        <v>3.26</v>
+      </c>
+      <c r="G64" s="2" t="n">
+        <v>0.4762</v>
+      </c>
+      <c r="H64" s="9" t="n">
+        <f aca="false">$F$58/(F64*$D64)</f>
+        <v>0.157975460122699</v>
+      </c>
+      <c r="I64" s="9" t="n">
+        <f aca="false">$G$58/(G64*$D64)</f>
+        <v>0.224170516589668</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="8" t="n">
+        <f aca="false">4000*4000</f>
+        <v>16000000</v>
+      </c>
+      <c r="C65" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>0.8074</v>
+      </c>
+      <c r="F65" s="2" t="n">
+        <v>82.88</v>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>13.37</v>
+      </c>
+      <c r="H65" s="9" t="n">
+        <f aca="false">$F$65/(F65*$D65)</f>
+        <v>1</v>
+      </c>
+      <c r="I65" s="9" t="n">
+        <f aca="false">$G$65/(G65*$D65)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="8" t="n">
+        <f aca="false">4000*4000</f>
+        <v>16000000</v>
+      </c>
+      <c r="C66" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>0.3915</v>
+      </c>
+      <c r="F66" s="2" t="n">
+        <v>44.05</v>
+      </c>
+      <c r="G66" s="2" t="n">
+        <v>7.103</v>
+      </c>
+      <c r="H66" s="9" t="n">
+        <f aca="false">$F$65/(F66*$D66)</f>
+        <v>0.940749148694665</v>
+      </c>
+      <c r="I66" s="9" t="n">
+        <f aca="false">$G$65/(G66*$D66)</f>
+        <v>0.94115162607349</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" s="8" t="n">
+        <f aca="false">4000*4000</f>
+        <v>16000000</v>
+      </c>
+      <c r="C67" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>0.323</v>
+      </c>
+      <c r="F67" s="2" t="n">
+        <v>26.94</v>
+      </c>
+      <c r="G67" s="2" t="n">
+        <v>3.375</v>
+      </c>
+      <c r="H67" s="9" t="n">
+        <f aca="false">$F$65/(F67*$D67)</f>
+        <v>0.769116555308092</v>
+      </c>
+      <c r="I67" s="9" t="n">
+        <f aca="false">$G$65/(G67*$D67)</f>
+        <v>0.99037037037037</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="8" t="n">
+        <f aca="false">4000*4000</f>
+        <v>16000000</v>
+      </c>
+      <c r="C68" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>0.3789</v>
+      </c>
+      <c r="F68" s="2" t="n">
+        <v>19.84</v>
+      </c>
+      <c r="G68" s="2" t="n">
+        <v>2.038</v>
+      </c>
+      <c r="H68" s="9" t="n">
+        <f aca="false">$F$65/(F68*$D68)</f>
+        <v>0.522177419354839</v>
+      </c>
+      <c r="I68" s="9" t="n">
+        <f aca="false">$G$65/(G68*$D68)</f>
+        <v>0.8200441609421</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="8" t="n">
+        <f aca="false">4000*4000</f>
+        <v>16000000</v>
+      </c>
+      <c r="C69" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>0.4608</v>
+      </c>
+      <c r="F69" s="2" t="n">
+        <v>18.56</v>
+      </c>
+      <c r="G69" s="2" t="n">
+        <v>1.433</v>
+      </c>
+      <c r="H69" s="9" t="n">
+        <f aca="false">$F$65/(F69*$D69)</f>
+        <v>0.446551724137931</v>
+      </c>
+      <c r="I69" s="9" t="n">
+        <f aca="false">$G$65/(G69*$D69)</f>
+        <v>0.933007676203768</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="8" t="n">
+        <f aca="false">4000*4000</f>
+        <v>16000000</v>
+      </c>
+      <c r="C70" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>0.4315</v>
+      </c>
+      <c r="F70" s="2" t="n">
+        <v>22.97</v>
+      </c>
+      <c r="G70" s="2" t="n">
+        <v>2.019</v>
+      </c>
+      <c r="H70" s="9" t="n">
+        <f aca="false">$F$65/(F70*$D70)</f>
+        <v>0.225511536787114</v>
+      </c>
+      <c r="I70" s="9" t="n">
+        <f aca="false">$G$65/(G70*$D70)</f>
+        <v>0.413880633977216</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="8" t="n">
+        <f aca="false">4000*4000</f>
+        <v>16000000</v>
+      </c>
+      <c r="C71" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="F71" s="2" t="n">
+        <v>26.55</v>
+      </c>
+      <c r="G71" s="2" t="n">
+        <v>1.552</v>
+      </c>
+      <c r="H71" s="9" t="n">
+        <f aca="false">$F$65/(F71*$D71)</f>
+        <v>0.15608286252354</v>
+      </c>
+      <c r="I71" s="9" t="n">
+        <f aca="false">$G$65/(G71*$D71)</f>
+        <v>0.430734536082474</v>
       </c>
     </row>
   </sheetData>
@@ -1890,17 +2571,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="16.4336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="17.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1023" min="11" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="6.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="16.4336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="16.7142857142857"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="17.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1023" min="11" style="8" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -1938,981 +2619,981 @@
       <c r="AMJ1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="n">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="n">
+      <c r="E2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="n">
         <v>6.373</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="8" t="n">
         <v>628.6</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="8" t="n">
         <v>100.5</v>
       </c>
-      <c r="I2" s="7" t="n">
+      <c r="I2" s="9" t="n">
         <f aca="false">$G$2/(G2*$E2)</f>
         <v>1</v>
       </c>
-      <c r="J2" s="7" t="n">
+      <c r="J2" s="9" t="n">
         <f aca="false">$H$2/(H2*$E2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="n">
+      <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="8" t="n">
         <v>3.222</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="8" t="n">
         <v>673.2</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="8" t="n">
         <v>52.29</v>
       </c>
-      <c r="I3" s="7" t="n">
+      <c r="I3" s="9" t="n">
         <f aca="false">$G$2/(G3*$E3)</f>
         <v>0.466874628639334</v>
       </c>
-      <c r="J3" s="7" t="n">
+      <c r="J3" s="9" t="n">
         <f aca="false">$H$2/(H3*$E3)</f>
         <v>0.960986804360298</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="n">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="8" t="n">
         <v>4.676</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="8" t="n">
         <v>391.4</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="8" t="n">
         <v>26.91</v>
       </c>
-      <c r="I4" s="7" t="n">
+      <c r="I4" s="9" t="n">
         <f aca="false">$G$2/(G4*$E4)</f>
         <v>0.401507409299949</v>
       </c>
-      <c r="J4" s="7" t="n">
+      <c r="J4" s="9" t="n">
         <f aca="false">$H$2/(H4*$E4)</f>
         <v>0.933667781493868</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="n">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="8" t="n">
         <v>4.611</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="8" t="n">
         <v>472.2</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="8" t="n">
         <v>14.64</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="9" t="n">
         <f aca="false">$G$2/(G5*$E5)</f>
         <v>0.16640194832698</v>
       </c>
-      <c r="J5" s="7" t="n">
+      <c r="J5" s="9" t="n">
         <f aca="false">$H$2/(H5*$E5)</f>
         <v>0.858094262295082</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="n">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="E6" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>6.21</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="8" t="n">
         <v>410.6</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="8" t="n">
         <v>11.83</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="9" t="n">
         <f aca="false">$G$2/(G6*$E6)</f>
         <v>0.153093034583536</v>
       </c>
-      <c r="J6" s="7" t="n">
+      <c r="J6" s="9" t="n">
         <f aca="false">$H$2/(H6*$E6)</f>
         <v>0.849535080304311</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="n">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="8" t="n">
         <v>2.258</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="8" t="n">
         <v>466.7</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="8" t="n">
         <v>15.33</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="9" t="n">
         <f aca="false">$G$2/(G7*$E7)</f>
         <v>0.0841814870366403</v>
       </c>
-      <c r="J7" s="7" t="n">
+      <c r="J7" s="9" t="n">
         <f aca="false">$H$2/(H7*$E7)</f>
         <v>0.409735812133072</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="n">
+      <c r="A8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="8" t="n">
         <v>1.8</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="8" t="n">
         <v>441.4</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="8" t="n">
         <v>12.84</v>
       </c>
-      <c r="I8" s="7" t="n">
+      <c r="I8" s="9" t="n">
         <f aca="false">$G$2/(G8*$E8)</f>
         <v>0.0712052560036248</v>
       </c>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="9" t="n">
         <f aca="false">$H$2/(H8*$E8)</f>
         <v>0.391355140186916</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="n">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="E9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8" t="n">
         <v>2.943</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="8" t="n">
         <v>628.6</v>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="8" t="n">
         <v>100.6</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I9" s="9" t="n">
         <f aca="false">$G$9/(G9*$E9)</f>
         <v>1</v>
       </c>
-      <c r="J9" s="7" t="n">
+      <c r="J9" s="9" t="n">
         <f aca="false">$H$9/(H9*$E9)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="n">
+      <c r="A10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="8" t="n">
         <v>4.396</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="8" t="n">
         <v>335.8</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="8" t="n">
         <v>51.24</v>
       </c>
-      <c r="I10" s="7" t="n">
+      <c r="I10" s="9" t="n">
         <f aca="false">$G$9/(G10*$E10)</f>
         <v>0.935973793924955</v>
       </c>
-      <c r="J10" s="7" t="n">
+      <c r="J10" s="9" t="n">
         <f aca="false">$H$9/(H10*$E10)</f>
         <v>0.981654957064793</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="n">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="8" t="n">
         <v>1.533</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="8" t="n">
         <v>193.8</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="8" t="n">
         <v>26.15</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="9" t="n">
         <f aca="false">$G$9/(G11*$E11)</f>
         <v>0.810887512899897</v>
       </c>
-      <c r="J11" s="7" t="n">
+      <c r="J11" s="9" t="n">
         <f aca="false">$H$9/(H11*$E11)</f>
         <v>0.961759082217973</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="n">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="8" t="n">
         <v>1.347</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="8" t="n">
         <v>140.3</v>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="H12" s="8" t="n">
         <v>13.17</v>
       </c>
-      <c r="I12" s="7" t="n">
+      <c r="I12" s="9" t="n">
         <f aca="false">$G$9/(G12*$E12)</f>
         <v>0.560049893086244</v>
       </c>
-      <c r="J12" s="7" t="n">
+      <c r="J12" s="9" t="n">
         <f aca="false">$H$9/(H12*$E12)</f>
         <v>0.954821564160972</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="n">
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2" t="n">
+      <c r="E13" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="8" t="n">
         <v>2.898</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="8" t="n">
         <v>130</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="8" t="n">
         <v>11.02</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="9" t="n">
         <f aca="false">$G$9/(G13*$E13)</f>
         <v>0.483538461538462</v>
       </c>
-      <c r="J13" s="7" t="n">
+      <c r="J13" s="9" t="n">
         <f aca="false">$H$9/(H13*$E13)</f>
         <v>0.912885662431942</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2" t="n">
+      <c r="A14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="8" t="n">
         <v>1.221</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="8" t="n">
         <v>191.1</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="8" t="n">
         <v>7.922</v>
       </c>
-      <c r="I14" s="7" t="n">
+      <c r="I14" s="9" t="n">
         <f aca="false">$G$9/(G14*$E14)</f>
         <v>0.205586080586081</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="9" t="n">
         <f aca="false">$H$9/(H14*$E14)</f>
         <v>0.793675839434486</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2" t="n">
+      <c r="A15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="8" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="8" t="n">
         <v>1.469</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="8" t="n">
         <v>238.4</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="H15" s="8" t="n">
         <v>8.245</v>
       </c>
-      <c r="I15" s="7" t="n">
+      <c r="I15" s="9" t="n">
         <f aca="false">$G$9/(G15*$E15)</f>
         <v>0.131837248322148</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="9" t="n">
         <f aca="false">$H$9/(H15*$E15)</f>
         <v>0.610066707095209</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="2" t="n">
+      <c r="A16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="n">
+      <c r="E16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8" t="n">
         <v>56.83</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="8" t="n">
         <v>5116</v>
       </c>
-      <c r="H16" s="2" t="n">
+      <c r="H16" s="8" t="n">
         <v>801.5</v>
       </c>
-      <c r="I16" s="7" t="n">
+      <c r="I16" s="9" t="n">
         <f aca="false">$G$16/(G16*$E16)</f>
         <v>1</v>
       </c>
-      <c r="J16" s="7" t="n">
+      <c r="J16" s="9" t="n">
         <f aca="false">$H$16/(H16*$E16)</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2" t="n">
+      <c r="A17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="8" t="n">
         <v>58.52</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="8" t="n">
         <v>4843</v>
       </c>
-      <c r="H17" s="2" t="n">
+      <c r="H17" s="8" t="n">
         <v>406</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I17" s="9" t="n">
         <f aca="false">$G$16/(G17*$E17)</f>
         <v>0.528185009291761</v>
       </c>
-      <c r="J17" s="7" t="n">
+      <c r="J17" s="9" t="n">
         <f aca="false">$H$16/(H17*$E17)</f>
         <v>0.987068965517241</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2" t="n">
+      <c r="A18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="8" t="n">
         <v>59.16</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="8" t="n">
         <v>4843</v>
       </c>
-      <c r="H18" s="2" t="n">
+      <c r="H18" s="8" t="n">
         <v>205.3</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I18" s="9" t="n">
         <f aca="false">$G$16/(G18*$E18)</f>
         <v>0.264092504645881</v>
       </c>
-      <c r="J18" s="7" t="n">
+      <c r="J18" s="9" t="n">
         <f aca="false">$H$16/(H18*$E18)</f>
         <v>0.976010716025329</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2" t="n">
+      <c r="A19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="8" t="n">
         <v>56.97</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G19" s="8" t="n">
         <v>2756</v>
       </c>
-      <c r="H19" s="2" t="n">
+      <c r="H19" s="8" t="n">
         <v>104.5</v>
       </c>
-      <c r="I19" s="7" t="n">
+      <c r="I19" s="9" t="n">
         <f aca="false">$G$16/(G19*$E19)</f>
         <v>0.232039187227866</v>
       </c>
-      <c r="J19" s="7" t="n">
+      <c r="J19" s="9" t="n">
         <f aca="false">$H$16/(H19*$E19)</f>
         <v>0.958732057416268</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="2" t="n">
+      <c r="A20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F20" s="2" t="n">
+      <c r="E20" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" s="8" t="n">
         <v>60.02</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G20" s="8" t="n">
         <v>3020</v>
       </c>
-      <c r="H20" s="2" t="n">
+      <c r="H20" s="8" t="n">
         <v>84.06</v>
       </c>
-      <c r="I20" s="7" t="n">
+      <c r="I20" s="9" t="n">
         <f aca="false">$G$16/(G20*$E20)</f>
         <v>0.169403973509934</v>
       </c>
-      <c r="J20" s="7" t="n">
+      <c r="J20" s="9" t="n">
         <f aca="false">$H$16/(H20*$E20)</f>
         <v>0.953485605519867</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2" t="n">
+      <c r="A21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="8" t="n">
         <v>57.73</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G21" s="8" t="n">
         <v>2370</v>
       </c>
-      <c r="H21" s="2" t="n">
+      <c r="H21" s="8" t="n">
         <v>61.7</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I21" s="9" t="n">
         <f aca="false">$G$16/(G21*$E21)</f>
         <v>0.134915611814346</v>
       </c>
-      <c r="J21" s="7" t="n">
+      <c r="J21" s="9" t="n">
         <f aca="false">$H$16/(H21*$E21)</f>
         <v>0.811892220421394</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="2" t="n">
+      <c r="A22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="8" t="n">
         <v>57.79</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="8" t="n">
         <v>1998</v>
       </c>
-      <c r="H22" s="2" t="n">
+      <c r="H22" s="8" t="n">
         <v>51.66</v>
       </c>
-      <c r="I22" s="7" t="n">
+      <c r="I22" s="9" t="n">
         <f aca="false">$G$16/(G22*$E22)</f>
         <v>0.128028028028028</v>
       </c>
-      <c r="J22" s="7" t="n">
+      <c r="J22" s="9" t="n">
         <f aca="false">$H$16/(H22*$E22)</f>
         <v>0.775745257452575</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="2" t="n">
+      <c r="A23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="n">
+      <c r="E23" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8" t="n">
         <v>57.26</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G23" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="H23" s="2" t="n">
+      <c r="H23" s="8" t="n">
         <v>802</v>
       </c>
-      <c r="I23" s="7" t="n">
+      <c r="I23" s="9" t="n">
         <f aca="false">$G$23/(G23*$E23)</f>
         <v>1</v>
       </c>
-      <c r="J23" s="7" t="n">
+      <c r="J23" s="9" t="n">
         <f aca="false">$H$23/(H23*$E23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="2" t="n">
+      <c r="A24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E24" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F24" s="8" t="n">
         <v>58.62</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G24" s="8" t="n">
         <v>2698</v>
       </c>
-      <c r="H24" s="2" t="n">
+      <c r="H24" s="8" t="n">
         <v>401.5</v>
       </c>
-      <c r="I24" s="7" t="n">
+      <c r="I24" s="9" t="n">
         <f aca="false">$G$23/(G24*$E24)</f>
         <v>0.94885100074129</v>
       </c>
-      <c r="J24" s="7" t="n">
+      <c r="J24" s="9" t="n">
         <f aca="false">$H$23/(H24*$E24)</f>
         <v>0.998754669987547</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="2" t="n">
+      <c r="A25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="8" t="n">
         <v>57.26</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="8" t="n">
         <v>1483</v>
       </c>
-      <c r="H25" s="2" t="n">
+      <c r="H25" s="8" t="n">
         <v>201.7</v>
       </c>
-      <c r="I25" s="7" t="n">
+      <c r="I25" s="9" t="n">
         <f aca="false">$G$23/(G25*$E25)</f>
         <v>0.863115306810519</v>
       </c>
-      <c r="J25" s="7" t="n">
+      <c r="J25" s="9" t="n">
         <f aca="false">$H$23/(H25*$E25)</f>
         <v>0.994050570153694</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="2" t="n">
+      <c r="A26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C26" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F26" s="8" t="n">
         <v>55.28</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="8" t="n">
         <v>1044</v>
       </c>
-      <c r="H26" s="2" t="n">
+      <c r="H26" s="8" t="n">
         <v>101.5</v>
       </c>
-      <c r="I26" s="7" t="n">
+      <c r="I26" s="9" t="n">
         <f aca="false">$G$23/(G26*$E26)</f>
         <v>0.613026819923372</v>
       </c>
-      <c r="J26" s="7" t="n">
+      <c r="J26" s="9" t="n">
         <f aca="false">$H$23/(H26*$E26)</f>
         <v>0.987684729064039</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="2" t="n">
+      <c r="A27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F27" s="2" t="n">
+      <c r="E27" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" s="8" t="n">
         <v>55.96</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="8" t="n">
         <v>967.5</v>
       </c>
-      <c r="H27" s="2" t="n">
+      <c r="H27" s="8" t="n">
         <v>81.76</v>
       </c>
-      <c r="I27" s="7" t="n">
+      <c r="I27" s="9" t="n">
         <f aca="false">$G$23/(G27*$E27)</f>
         <v>0.529198966408269</v>
       </c>
-      <c r="J27" s="7" t="n">
+      <c r="J27" s="9" t="n">
         <f aca="false">$H$23/(H27*$E27)</f>
         <v>0.980919765166341</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="2" t="n">
+      <c r="A28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="2" t="n">
+      <c r="E28" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F28" s="8" t="n">
         <v>55.9</v>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G28" s="8" t="n">
         <v>1539</v>
       </c>
-      <c r="H28" s="2" t="n">
+      <c r="H28" s="8" t="n">
         <v>52.99</v>
       </c>
-      <c r="I28" s="7" t="n">
+      <c r="I28" s="9" t="n">
         <f aca="false">$G$23/(G28*$E28)</f>
         <v>0.207927225471085</v>
       </c>
-      <c r="J28" s="7" t="n">
+      <c r="J28" s="9" t="n">
         <f aca="false">$H$23/(H28*$E28)</f>
         <v>0.945933194942442</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="2" t="n">
+      <c r="A29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="8" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C29" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="2" t="n">
+      <c r="E29" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F29" s="8" t="n">
         <v>55.73</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G29" s="8" t="n">
         <v>1948</v>
       </c>
-      <c r="H29" s="2" t="n">
+      <c r="H29" s="8" t="n">
         <v>48.79</v>
       </c>
-      <c r="I29" s="7" t="n">
+      <c r="I29" s="9" t="n">
         <f aca="false">$G$23/(G29*$E29)</f>
         <v>0.131416837782341</v>
       </c>
-      <c r="J29" s="7" t="n">
+      <c r="J29" s="9" t="n">
         <f aca="false">$H$23/(H29*$E29)</f>
         <v>0.821889731502357</v>
       </c>

</xml_diff>

<commit_message>
Added more benchmark results
</commit_message>
<xml_diff>
--- a/Math/Lapack/SVD/svd_benchmarks.xlsx
+++ b/Math/Lapack/SVD/svd_benchmarks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="749" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="749" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="scaling" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="27">
   <si>
     <t>cluster</t>
   </si>
@@ -248,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,11 +285,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,6 +306,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,10 +356,10 @@
   </sheetPr>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="600" topLeftCell="A4" activePane="bottomLeft" state="split"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="600" topLeftCell="A55" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3167,981 +3175,981 @@
       <c r="AMJ1" s="14"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="10" t="n">
+      <c r="A2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10" t="n">
+      <c r="E2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="16" t="n">
         <v>6.373</v>
       </c>
-      <c r="G2" s="10" t="n">
+      <c r="G2" s="16" t="n">
         <v>628.6</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="16" t="n">
         <v>100.5</v>
       </c>
-      <c r="I2" s="15" t="n">
+      <c r="I2" s="17" t="n">
         <f aca="false">$G$2/(G2*$E2)</f>
         <v>1</v>
       </c>
-      <c r="J2" s="15" t="n">
+      <c r="J2" s="17" t="n">
         <f aca="false">$H$2/(H2*$E2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="10" t="n">
+      <c r="A3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="10" t="n">
+      <c r="E3" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="F3" s="16" t="n">
         <v>3.222</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="16" t="n">
         <v>673.2</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="16" t="n">
         <v>52.29</v>
       </c>
-      <c r="I3" s="15" t="n">
+      <c r="I3" s="17" t="n">
         <f aca="false">$G$2/(G3*$E3)</f>
         <v>0.466874628639334</v>
       </c>
-      <c r="J3" s="15" t="n">
+      <c r="J3" s="17" t="n">
         <f aca="false">$H$2/(H3*$E3)</f>
         <v>0.960986804360298</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="10" t="n">
+      <c r="A4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E4" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="F4" s="16" t="n">
         <v>4.676</v>
       </c>
-      <c r="G4" s="10" t="n">
+      <c r="G4" s="16" t="n">
         <v>391.4</v>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="H4" s="16" t="n">
         <v>26.91</v>
       </c>
-      <c r="I4" s="15" t="n">
+      <c r="I4" s="17" t="n">
         <f aca="false">$G$2/(G4*$E4)</f>
         <v>0.401507409299949</v>
       </c>
-      <c r="J4" s="15" t="n">
+      <c r="J4" s="17" t="n">
         <f aca="false">$H$2/(H4*$E4)</f>
         <v>0.933667781493868</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="10" t="n">
+      <c r="A5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="10" t="n">
+      <c r="E5" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="16" t="n">
         <v>4.611</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="G5" s="16" t="n">
         <v>472.2</v>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="H5" s="16" t="n">
         <v>14.64</v>
       </c>
-      <c r="I5" s="15" t="n">
+      <c r="I5" s="17" t="n">
         <f aca="false">$G$2/(G5*$E5)</f>
         <v>0.16640194832698</v>
       </c>
-      <c r="J5" s="15" t="n">
+      <c r="J5" s="17" t="n">
         <f aca="false">$H$2/(H5*$E5)</f>
         <v>0.858094262295082</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="10" t="n">
+      <c r="A6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" s="10" t="n">
+      <c r="E6" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="16" t="n">
         <v>6.21</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="16" t="n">
         <v>410.6</v>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="H6" s="16" t="n">
         <v>11.83</v>
       </c>
-      <c r="I6" s="15" t="n">
+      <c r="I6" s="17" t="n">
         <f aca="false">$G$2/(G6*$E6)</f>
         <v>0.153093034583536</v>
       </c>
-      <c r="J6" s="15" t="n">
+      <c r="J6" s="17" t="n">
         <f aca="false">$H$2/(H6*$E6)</f>
         <v>0.849535080304311</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="10" t="n">
+      <c r="A7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C7" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="10" t="n">
+      <c r="E7" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="F7" s="16" t="n">
         <v>2.258</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="G7" s="16" t="n">
         <v>466.7</v>
       </c>
-      <c r="H7" s="10" t="n">
+      <c r="H7" s="16" t="n">
         <v>15.33</v>
       </c>
-      <c r="I7" s="15" t="n">
+      <c r="I7" s="17" t="n">
         <f aca="false">$G$2/(G7*$E7)</f>
         <v>0.0841814870366403</v>
       </c>
-      <c r="J7" s="15" t="n">
+      <c r="J7" s="17" t="n">
         <f aca="false">$H$2/(H7*$E7)</f>
         <v>0.409735812133072</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="10" t="n">
+      <c r="A8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="10" t="n">
+      <c r="E8" s="16" t="n">
         <v>20</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="16" t="n">
         <v>1.8</v>
       </c>
-      <c r="G8" s="10" t="n">
+      <c r="G8" s="16" t="n">
         <v>441.4</v>
       </c>
-      <c r="H8" s="10" t="n">
+      <c r="H8" s="16" t="n">
         <v>12.84</v>
       </c>
-      <c r="I8" s="15" t="n">
+      <c r="I8" s="17" t="n">
         <f aca="false">$G$2/(G8*$E8)</f>
         <v>0.0712052560036248</v>
       </c>
-      <c r="J8" s="15" t="n">
+      <c r="J8" s="17" t="n">
         <f aca="false">$H$2/(H8*$E8)</f>
         <v>0.391355140186916</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="10" t="n">
+      <c r="A9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10" t="n">
+      <c r="E9" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16" t="n">
         <v>2.943</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="G9" s="16" t="n">
         <v>628.6</v>
       </c>
-      <c r="H9" s="10" t="n">
+      <c r="H9" s="16" t="n">
         <v>100.6</v>
       </c>
-      <c r="I9" s="15" t="n">
+      <c r="I9" s="17" t="n">
         <f aca="false">$G$9/(G9*$E9)</f>
         <v>1</v>
       </c>
-      <c r="J9" s="15" t="n">
+      <c r="J9" s="17" t="n">
         <f aca="false">$H$9/(H9*$E9)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="10" t="n">
+      <c r="A10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="10" t="n">
+      <c r="E10" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="10" t="n">
+      <c r="F10" s="16" t="n">
         <v>4.396</v>
       </c>
-      <c r="G10" s="10" t="n">
+      <c r="G10" s="16" t="n">
         <v>335.8</v>
       </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="16" t="n">
         <v>51.24</v>
       </c>
-      <c r="I10" s="15" t="n">
+      <c r="I10" s="17" t="n">
         <f aca="false">$G$9/(G10*$E10)</f>
         <v>0.935973793924955</v>
       </c>
-      <c r="J10" s="15" t="n">
+      <c r="J10" s="17" t="n">
         <f aca="false">$H$9/(H10*$E10)</f>
         <v>0.981654957064793</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="10" t="n">
+      <c r="A11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C11" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="10" t="n">
+      <c r="E11" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F11" s="10" t="n">
+      <c r="F11" s="16" t="n">
         <v>1.533</v>
       </c>
-      <c r="G11" s="10" t="n">
+      <c r="G11" s="16" t="n">
         <v>193.8</v>
       </c>
-      <c r="H11" s="10" t="n">
+      <c r="H11" s="16" t="n">
         <v>26.15</v>
       </c>
-      <c r="I11" s="15" t="n">
+      <c r="I11" s="17" t="n">
         <f aca="false">$G$9/(G11*$E11)</f>
         <v>0.810887512899897</v>
       </c>
-      <c r="J11" s="15" t="n">
+      <c r="J11" s="17" t="n">
         <f aca="false">$H$9/(H11*$E11)</f>
         <v>0.961759082217973</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="10" t="n">
+      <c r="A12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="10" t="n">
+      <c r="E12" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="F12" s="16" t="n">
         <v>1.347</v>
       </c>
-      <c r="G12" s="10" t="n">
+      <c r="G12" s="16" t="n">
         <v>140.3</v>
       </c>
-      <c r="H12" s="10" t="n">
+      <c r="H12" s="16" t="n">
         <v>13.17</v>
       </c>
-      <c r="I12" s="15" t="n">
+      <c r="I12" s="17" t="n">
         <f aca="false">$G$9/(G12*$E12)</f>
         <v>0.560049893086244</v>
       </c>
-      <c r="J12" s="15" t="n">
+      <c r="J12" s="17" t="n">
         <f aca="false">$H$9/(H12*$E12)</f>
         <v>0.954821564160972</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="10" t="n">
+      <c r="A13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C13" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F13" s="10" t="n">
+      <c r="E13" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="16" t="n">
         <v>2.898</v>
       </c>
-      <c r="G13" s="10" t="n">
+      <c r="G13" s="16" t="n">
         <v>130</v>
       </c>
-      <c r="H13" s="10" t="n">
+      <c r="H13" s="16" t="n">
         <v>11.02</v>
       </c>
-      <c r="I13" s="15" t="n">
+      <c r="I13" s="17" t="n">
         <f aca="false">$G$9/(G13*$E13)</f>
         <v>0.483538461538462</v>
       </c>
-      <c r="J13" s="15" t="n">
+      <c r="J13" s="17" t="n">
         <f aca="false">$H$9/(H13*$E13)</f>
         <v>0.912885662431942</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="10" t="n">
+      <c r="A14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C14" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="E14" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="16" t="n">
         <v>1.221</v>
       </c>
-      <c r="G14" s="10" t="n">
+      <c r="G14" s="16" t="n">
         <v>191.1</v>
       </c>
-      <c r="H14" s="10" t="n">
+      <c r="H14" s="16" t="n">
         <v>7.922</v>
       </c>
-      <c r="I14" s="15" t="n">
+      <c r="I14" s="17" t="n">
         <f aca="false">$G$9/(G14*$E14)</f>
         <v>0.205586080586081</v>
       </c>
-      <c r="J14" s="15" t="n">
+      <c r="J14" s="17" t="n">
         <f aca="false">$H$9/(H14*$E14)</f>
         <v>0.793675839434486</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="n">
+      <c r="A15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="n">
         <f aca="false">8000*8000</f>
         <v>64000000</v>
       </c>
-      <c r="C15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="10" t="n">
+      <c r="E15" s="16" t="n">
         <v>20</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="F15" s="16" t="n">
         <v>1.469</v>
       </c>
-      <c r="G15" s="10" t="n">
+      <c r="G15" s="16" t="n">
         <v>238.4</v>
       </c>
-      <c r="H15" s="10" t="n">
+      <c r="H15" s="16" t="n">
         <v>8.245</v>
       </c>
-      <c r="I15" s="15" t="n">
+      <c r="I15" s="17" t="n">
         <f aca="false">$G$9/(G15*$E15)</f>
         <v>0.131837248322148</v>
       </c>
-      <c r="J15" s="15" t="n">
+      <c r="J15" s="17" t="n">
         <f aca="false">$H$9/(H15*$E15)</f>
         <v>0.610066707095209</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="10" t="n">
+      <c r="A16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C16" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="10" t="n">
+      <c r="E16" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="16" t="n">
         <v>56.83</v>
       </c>
-      <c r="G16" s="10" t="n">
+      <c r="G16" s="16" t="n">
         <v>5116</v>
       </c>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="16" t="n">
         <v>801.5</v>
       </c>
-      <c r="I16" s="15" t="n">
+      <c r="I16" s="17" t="n">
         <f aca="false">$G$16/(G16*$E16)</f>
         <v>1</v>
       </c>
-      <c r="J16" s="15" t="n">
+      <c r="J16" s="17" t="n">
         <f aca="false">$H$16/(H16*$E16)</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="10" t="n">
+      <c r="A17" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C17" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="C17" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="E17" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="16" t="n">
         <v>58.52</v>
       </c>
-      <c r="G17" s="10" t="n">
+      <c r="G17" s="16" t="n">
         <v>4843</v>
       </c>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="16" t="n">
         <v>406</v>
       </c>
-      <c r="I17" s="15" t="n">
+      <c r="I17" s="17" t="n">
         <f aca="false">$G$16/(G17*$E17)</f>
         <v>0.528185009291761</v>
       </c>
-      <c r="J17" s="15" t="n">
+      <c r="J17" s="17" t="n">
         <f aca="false">$H$16/(H17*$E17)</f>
         <v>0.987068965517241</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="10" t="n">
+      <c r="A18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="10" t="n">
+      <c r="E18" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F18" s="10" t="n">
+      <c r="F18" s="16" t="n">
         <v>59.16</v>
       </c>
-      <c r="G18" s="10" t="n">
+      <c r="G18" s="16" t="n">
         <v>4843</v>
       </c>
-      <c r="H18" s="10" t="n">
+      <c r="H18" s="16" t="n">
         <v>205.3</v>
       </c>
-      <c r="I18" s="15" t="n">
+      <c r="I18" s="17" t="n">
         <f aca="false">$G$16/(G18*$E18)</f>
         <v>0.264092504645881</v>
       </c>
-      <c r="J18" s="15" t="n">
+      <c r="J18" s="17" t="n">
         <f aca="false">$H$16/(H18*$E18)</f>
         <v>0.976010716025329</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="10" t="n">
+      <c r="A19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C19" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="C19" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="10" t="n">
+      <c r="E19" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="F19" s="10" t="n">
+      <c r="F19" s="16" t="n">
         <v>56.97</v>
       </c>
-      <c r="G19" s="10" t="n">
+      <c r="G19" s="16" t="n">
         <v>2756</v>
       </c>
-      <c r="H19" s="10" t="n">
+      <c r="H19" s="16" t="n">
         <v>104.5</v>
       </c>
-      <c r="I19" s="15" t="n">
+      <c r="I19" s="17" t="n">
         <f aca="false">$G$16/(G19*$E19)</f>
         <v>0.232039187227866</v>
       </c>
-      <c r="J19" s="15" t="n">
+      <c r="J19" s="17" t="n">
         <f aca="false">$H$16/(H19*$E19)</f>
         <v>0.958732057416268</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="10" t="n">
+      <c r="A20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C20" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F20" s="10" t="n">
+      <c r="E20" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" s="16" t="n">
         <v>60.02</v>
       </c>
-      <c r="G20" s="10" t="n">
+      <c r="G20" s="16" t="n">
         <v>3020</v>
       </c>
-      <c r="H20" s="10" t="n">
+      <c r="H20" s="16" t="n">
         <v>84.06</v>
       </c>
-      <c r="I20" s="15" t="n">
+      <c r="I20" s="17" t="n">
         <f aca="false">$G$16/(G20*$E20)</f>
         <v>0.169403973509934</v>
       </c>
-      <c r="J20" s="15" t="n">
+      <c r="J20" s="17" t="n">
         <f aca="false">$H$16/(H20*$E20)</f>
         <v>0.953485605519867</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="10" t="n">
+      <c r="A21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C21" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="E21" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="F21" s="10" t="n">
+      <c r="F21" s="16" t="n">
         <v>57.73</v>
       </c>
-      <c r="G21" s="10" t="n">
+      <c r="G21" s="16" t="n">
         <v>2370</v>
       </c>
-      <c r="H21" s="10" t="n">
+      <c r="H21" s="16" t="n">
         <v>61.7</v>
       </c>
-      <c r="I21" s="15" t="n">
+      <c r="I21" s="17" t="n">
         <f aca="false">$G$16/(G21*$E21)</f>
         <v>0.134915611814346</v>
       </c>
-      <c r="J21" s="15" t="n">
+      <c r="J21" s="17" t="n">
         <f aca="false">$H$16/(H21*$E21)</f>
         <v>0.811892220421394</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="10" t="n">
+      <c r="A22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C22" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="C22" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="10" t="n">
+      <c r="E22" s="16" t="n">
         <v>20</v>
       </c>
-      <c r="F22" s="10" t="n">
+      <c r="F22" s="16" t="n">
         <v>57.79</v>
       </c>
-      <c r="G22" s="10" t="n">
+      <c r="G22" s="16" t="n">
         <v>1998</v>
       </c>
-      <c r="H22" s="10" t="n">
+      <c r="H22" s="16" t="n">
         <v>51.66</v>
       </c>
-      <c r="I22" s="15" t="n">
+      <c r="I22" s="17" t="n">
         <f aca="false">$G$16/(G22*$E22)</f>
         <v>0.128028028028028</v>
       </c>
-      <c r="J22" s="15" t="n">
+      <c r="J22" s="17" t="n">
         <f aca="false">$H$16/(H22*$E22)</f>
         <v>0.775745257452575</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="10" t="n">
+      <c r="A23" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C23" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="10" t="n">
+      <c r="E23" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16" t="n">
         <v>57.26</v>
       </c>
-      <c r="G23" s="10" t="n">
+      <c r="G23" s="16" t="n">
         <v>5120</v>
       </c>
-      <c r="H23" s="10" t="n">
+      <c r="H23" s="16" t="n">
         <v>802</v>
       </c>
-      <c r="I23" s="15" t="n">
+      <c r="I23" s="17" t="n">
         <f aca="false">$G$23/(G23*$E23)</f>
         <v>1</v>
       </c>
-      <c r="J23" s="15" t="n">
+      <c r="J23" s="17" t="n">
         <f aca="false">$H$23/(H23*$E23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="10" t="n">
+      <c r="A24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C24" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="C24" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="10" t="n">
+      <c r="E24" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="10" t="n">
+      <c r="F24" s="16" t="n">
         <v>58.62</v>
       </c>
-      <c r="G24" s="10" t="n">
+      <c r="G24" s="16" t="n">
         <v>2698</v>
       </c>
-      <c r="H24" s="10" t="n">
+      <c r="H24" s="16" t="n">
         <v>401.5</v>
       </c>
-      <c r="I24" s="15" t="n">
+      <c r="I24" s="17" t="n">
         <f aca="false">$G$23/(G24*$E24)</f>
         <v>0.94885100074129</v>
       </c>
-      <c r="J24" s="15" t="n">
+      <c r="J24" s="17" t="n">
         <f aca="false">$H$23/(H24*$E24)</f>
         <v>0.998754669987547</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="10" t="n">
+      <c r="A25" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C25" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C25" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="10" t="n">
+      <c r="E25" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F25" s="10" t="n">
+      <c r="F25" s="16" t="n">
         <v>57.26</v>
       </c>
-      <c r="G25" s="10" t="n">
+      <c r="G25" s="16" t="n">
         <v>1483</v>
       </c>
-      <c r="H25" s="10" t="n">
+      <c r="H25" s="16" t="n">
         <v>201.7</v>
       </c>
-      <c r="I25" s="15" t="n">
+      <c r="I25" s="17" t="n">
         <f aca="false">$G$23/(G25*$E25)</f>
         <v>0.863115306810519</v>
       </c>
-      <c r="J25" s="15" t="n">
+      <c r="J25" s="17" t="n">
         <f aca="false">$H$23/(H25*$E25)</f>
         <v>0.994050570153694</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="10" t="n">
+      <c r="A26" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C26" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="10" t="n">
+      <c r="E26" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="F26" s="10" t="n">
+      <c r="F26" s="16" t="n">
         <v>55.28</v>
       </c>
-      <c r="G26" s="10" t="n">
+      <c r="G26" s="16" t="n">
         <v>1044</v>
       </c>
-      <c r="H26" s="10" t="n">
+      <c r="H26" s="16" t="n">
         <v>101.5</v>
       </c>
-      <c r="I26" s="15" t="n">
+      <c r="I26" s="17" t="n">
         <f aca="false">$G$23/(G26*$E26)</f>
         <v>0.613026819923372</v>
       </c>
-      <c r="J26" s="15" t="n">
+      <c r="J26" s="17" t="n">
         <f aca="false">$H$23/(H26*$E26)</f>
         <v>0.987684729064039</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="10" t="n">
+      <c r="A27" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C27" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="C27" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F27" s="10" t="n">
+      <c r="E27" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" s="16" t="n">
         <v>55.96</v>
       </c>
-      <c r="G27" s="10" t="n">
+      <c r="G27" s="16" t="n">
         <v>967.5</v>
       </c>
-      <c r="H27" s="10" t="n">
+      <c r="H27" s="16" t="n">
         <v>81.76</v>
       </c>
-      <c r="I27" s="15" t="n">
+      <c r="I27" s="17" t="n">
         <f aca="false">$G$23/(G27*$E27)</f>
         <v>0.529198966408269</v>
       </c>
-      <c r="J27" s="15" t="n">
+      <c r="J27" s="17" t="n">
         <f aca="false">$H$23/(H27*$E27)</f>
         <v>0.980919765166341</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="10" t="n">
+      <c r="A28" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C28" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="C28" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="10" t="n">
+      <c r="E28" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="F28" s="10" t="n">
+      <c r="F28" s="16" t="n">
         <v>55.9</v>
       </c>
-      <c r="G28" s="10" t="n">
+      <c r="G28" s="16" t="n">
         <v>1539</v>
       </c>
-      <c r="H28" s="10" t="n">
+      <c r="H28" s="16" t="n">
         <v>52.99</v>
       </c>
-      <c r="I28" s="15" t="n">
+      <c r="I28" s="17" t="n">
         <f aca="false">$G$23/(G28*$E28)</f>
         <v>0.207927225471085</v>
       </c>
-      <c r="J28" s="15" t="n">
+      <c r="J28" s="17" t="n">
         <f aca="false">$H$23/(H28*$E28)</f>
         <v>0.945933194942442</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="10" t="n">
+      <c r="A29" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="16" t="n">
         <f aca="false">16000*16000</f>
         <v>256000000</v>
       </c>
-      <c r="C29" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="C29" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="16" t="n">
         <v>20</v>
       </c>
-      <c r="F29" s="10" t="n">
+      <c r="F29" s="16" t="n">
         <v>55.73</v>
       </c>
-      <c r="G29" s="10" t="n">
+      <c r="G29" s="16" t="n">
         <v>1948</v>
       </c>
-      <c r="H29" s="10" t="n">
+      <c r="H29" s="16" t="n">
         <v>48.79</v>
       </c>
-      <c r="I29" s="15" t="n">
+      <c r="I29" s="17" t="n">
         <f aca="false">$G$23/(G29*$E29)</f>
         <v>0.131416837782341</v>
       </c>
-      <c r="J29" s="15" t="n">
+      <c r="J29" s="17" t="n">
         <f aca="false">$H$23/(H29*$E29)</f>
         <v>0.821889731502357</v>
       </c>
@@ -4162,10 +4170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4174,319 +4182,384 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.43367346938776"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.01020408163265"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.90816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.76530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.93877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.76530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.93877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.0459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+    <row r="1" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="19" t="n">
+      <c r="A2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="D2" s="19" t="n">
+      <c r="D2" s="21" t="n">
         <f aca="false">B2*C2</f>
         <v>16</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="21" t="n">
         <v>4000</v>
       </c>
-      <c r="F2" s="19" t="n">
+      <c r="G2" s="21" t="n">
         <v>16000</v>
       </c>
-      <c r="G2" s="18" t="n">
+      <c r="H2" s="20" t="n">
         <v>41.71</v>
       </c>
-      <c r="H2" s="18" t="n">
+      <c r="I2" s="20" t="n">
         <v>2869</v>
       </c>
-      <c r="I2" s="18" t="n">
+      <c r="J2" s="20" t="n">
         <v>116.6</v>
       </c>
-      <c r="J2" s="7" t="n">
+      <c r="K2" s="7" t="n">
         <v>36.39</v>
       </c>
-      <c r="K2" s="7" t="n">
+      <c r="L2" s="7" t="n">
         <v>874.7</v>
       </c>
-      <c r="L2" s="7" t="n">
+      <c r="M2" s="7" t="n">
         <v>45.05</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="19" t="n">
+      <c r="A3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="D3" s="19" t="n">
+      <c r="D3" s="21" t="n">
         <f aca="false">B3*C3</f>
         <v>16</v>
       </c>
-      <c r="E3" s="19" t="n">
+      <c r="E3" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="21" t="n">
         <v>2000</v>
       </c>
-      <c r="F3" s="19" t="n">
+      <c r="G3" s="21" t="n">
         <v>16000</v>
       </c>
-      <c r="G3" s="18" t="n">
+      <c r="H3" s="20" t="n">
         <v>57.41</v>
       </c>
-      <c r="H3" s="18" t="n">
+      <c r="I3" s="20" t="n">
         <v>1897</v>
       </c>
-      <c r="I3" s="18" t="n">
+      <c r="J3" s="20" t="n">
         <v>116.2</v>
       </c>
-      <c r="J3" s="7" t="n">
+      <c r="K3" s="7" t="n">
         <v>36.39</v>
       </c>
-      <c r="K3" s="7" t="n">
+      <c r="L3" s="7" t="n">
         <v>874.7</v>
       </c>
-      <c r="L3" s="7" t="n">
+      <c r="M3" s="7" t="n">
         <v>45.05</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="19" t="n">
+      <c r="A4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="D4" s="19" t="n">
+      <c r="D4" s="21" t="n">
         <f aca="false">B4*C4</f>
         <v>16</v>
       </c>
-      <c r="E4" s="19" t="n">
+      <c r="E4" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21" t="n">
         <v>1000</v>
       </c>
-      <c r="F4" s="19" t="n">
+      <c r="G4" s="21" t="n">
         <v>16000</v>
       </c>
-      <c r="G4" s="18" t="n">
+      <c r="H4" s="20" t="n">
         <v>55.79</v>
       </c>
-      <c r="H4" s="18" t="n">
+      <c r="I4" s="20" t="n">
         <v>1467</v>
       </c>
-      <c r="I4" s="18" t="n">
+      <c r="J4" s="20" t="n">
         <v>116.3</v>
       </c>
-      <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="19" t="n">
+      <c r="A5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="D5" s="19" t="n">
+      <c r="D5" s="21" t="n">
         <f aca="false">B5*C5</f>
         <v>16</v>
       </c>
-      <c r="E5" s="19" t="n">
+      <c r="E5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="21" t="n">
         <v>500</v>
       </c>
-      <c r="F5" s="19" t="n">
+      <c r="G5" s="21" t="n">
         <v>16000</v>
       </c>
-      <c r="G5" s="18" t="n">
+      <c r="H5" s="20" t="n">
         <v>66.7</v>
       </c>
-      <c r="H5" s="18" t="n">
+      <c r="I5" s="20" t="n">
         <v>1279</v>
       </c>
-      <c r="I5" s="18" t="n">
+      <c r="J5" s="20" t="n">
         <v>115.8</v>
       </c>
-      <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="19" t="n">
+      <c r="A6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="D6" s="19" t="n">
+      <c r="D6" s="21" t="n">
         <f aca="false">B6*C6</f>
         <v>16</v>
       </c>
-      <c r="E6" s="19" t="n">
+      <c r="E6" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21" t="n">
         <v>64</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="G6" s="21" t="n">
         <v>16000</v>
       </c>
-      <c r="G6" s="18" t="n">
+      <c r="H6" s="20" t="n">
         <v>12.82</v>
       </c>
-      <c r="H6" s="18" t="n">
+      <c r="I6" s="20" t="n">
         <v>1212</v>
       </c>
-      <c r="I6" s="18" t="n">
+      <c r="J6" s="20" t="n">
         <v>123.8</v>
       </c>
-      <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="19" t="n">
+      <c r="A7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="D7" s="19" t="n">
+      <c r="D7" s="21" t="n">
         <f aca="false">B7*C7</f>
         <v>16</v>
       </c>
-      <c r="E7" s="19" t="n">
+      <c r="E7" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="21" t="n">
         <v>2000</v>
       </c>
-      <c r="F7" s="19" t="n">
+      <c r="G7" s="21" t="n">
         <v>8000</v>
       </c>
-      <c r="G7" s="18" t="n">
+      <c r="H7" s="20" t="n">
         <v>0.1571</v>
       </c>
-      <c r="H7" s="18" t="n">
+      <c r="I7" s="20" t="n">
         <v>401.4</v>
       </c>
-      <c r="I7" s="18" t="n">
+      <c r="J7" s="20" t="n">
         <v>16.64</v>
       </c>
-      <c r="J7" s="6" t="n">
+      <c r="K7" s="6" t="n">
         <v>1.221</v>
       </c>
-      <c r="K7" s="6" t="n">
+      <c r="L7" s="6" t="n">
         <v>191.1</v>
       </c>
-      <c r="L7" s="6" t="n">
+      <c r="M7" s="6" t="n">
         <v>7.922</v>
       </c>
-      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="19" t="n">
+      <c r="A8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="19" t="n">
+      <c r="C8" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="D8" s="19" t="n">
+      <c r="D8" s="21" t="n">
         <f aca="false">B8*C8</f>
         <v>64</v>
       </c>
-      <c r="E8" s="19" t="n">
+      <c r="E8" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="21" t="n">
         <v>4000</v>
       </c>
-      <c r="F8" s="19" t="n">
+      <c r="G8" s="21" t="n">
         <v>64000</v>
       </c>
-      <c r="G8" s="18" t="n">
-        <v>474.2</v>
-      </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
+      <c r="H8" s="20" t="n">
+        <v>481.9</v>
+      </c>
+      <c r="I8" s="20" t="n">
+        <v>16546</v>
+      </c>
+      <c r="J8" s="20" t="n">
+        <v>1842</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="19" t="n">
+      <c r="A9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="D9" s="19" t="n">
+      <c r="D9" s="21" t="n">
         <f aca="false">B9*C9</f>
         <v>16</v>
       </c>
-      <c r="E9" s="19" t="n">
+      <c r="E9" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="21" t="n">
         <v>64</v>
       </c>
-      <c r="F9" s="19" t="n">
+      <c r="G9" s="21" t="n">
         <v>32000</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>190.4</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>7213</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>933.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="21" t="n">
+        <f aca="false">B10*C10</f>
+        <v>4</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>64000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added benchmark results for Scalapack
</commit_message>
<xml_diff>
--- a/Math/Lapack/SVD/svd_benchmarks.xlsx
+++ b/Math/Lapack/SVD/svd_benchmarks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="27">
   <si>
     <t>cluster</t>
   </si>
@@ -357,9 +357,9 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="600" topLeftCell="A55" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="600" topLeftCell="A10" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4170,10 +4170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4561,6 +4561,42 @@
       <c r="G10" s="0" t="n">
         <v>64000</v>
       </c>
+      <c r="H10" s="0" t="n">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="21" t="n">
+        <f aca="false">B11*C11</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>110.9</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>388.6</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>16.32</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added Python benchmark results
</commit_message>
<xml_diff>
--- a/Math/Lapack/SVD/svd_benchmarks.xlsx
+++ b/Math/Lapack/SVD/svd_benchmarks.xlsx
@@ -5,19 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="749" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="749" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="scaling" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="effect_dplace" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="scalapack" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="python" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="35">
   <si>
     <t>cluster</t>
   </si>
@@ -98,6 +99,30 @@
   </si>
   <si>
     <t>pdgemm 1 &amp; 2 (s)</t>
+  </si>
+  <si>
+    <t>BLAS</t>
+  </si>
+  <si>
+    <t>linalg.svd (s)</t>
+  </si>
+  <si>
+    <t>np.dot 1 &amp; 2 (s)</t>
+  </si>
+  <si>
+    <t>linalg.svd efficiency</t>
+  </si>
+  <si>
+    <t>np.dot efficiency</t>
+  </si>
+  <si>
+    <t>svd ratio</t>
+  </si>
+  <si>
+    <t>dot ratio</t>
+  </si>
+  <si>
+    <t>intel</t>
   </si>
 </sst>
 </file>
@@ -248,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,6 +362,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -357,9 +386,9 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="600" topLeftCell="A10" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+      <pane xSplit="0" ySplit="600" topLeftCell="A13" activePane="topLeft" state="split"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1140,7 +1169,7 @@
       </c>
       <c r="J22" s="7" t="n">
         <f aca="false">$H$16/(H22*$E22)</f>
-        <v>0.617769376181474</v>
+        <v>0.617769376181475</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,7 +1900,7 @@
       </c>
       <c r="I43" s="7" t="n">
         <f aca="false">$H$16/(H22*$E43)</f>
-        <v>0.617769376181474</v>
+        <v>0.617769376181475</v>
       </c>
       <c r="J43" s="7" t="n">
         <f aca="false">$I$16/(I22*$E43)</f>
@@ -4172,7 +4201,7 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -4607,4 +4636,495 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.82142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="5.46428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.95408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.8826530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.8571428571429"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.07142857142857"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">C2*C2</f>
+        <v>64000000</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>516.9</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>76.38</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <f aca="false">$G$2/(G2*$F2)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="7" t="n">
+        <f aca="false">$H$2/(H2*$F2)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="6" t="n">
+        <v>526.8</v>
+      </c>
+      <c r="L2" s="6" t="n">
+        <v>75.99</v>
+      </c>
+      <c r="M2" s="7" t="n">
+        <f aca="false">$K$2/(K2*$F2)</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="7" t="n">
+        <f aca="false">$L$2/(L2*$F2)</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="22" t="n">
+        <f aca="false">G2/K2</f>
+        <v>0.98120728929385</v>
+      </c>
+      <c r="P2" s="22" t="n">
+        <f aca="false">H2/L2</f>
+        <v>1.00513225424398</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">C3*C3</f>
+        <v>64000000</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>365.3</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>38.79</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <f aca="false">$G$2/(G3*$F3)</f>
+        <v>0.707500684369012</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <f aca="false">$H$2/(H3*$F3)</f>
+        <v>0.984532095901005</v>
+      </c>
+      <c r="K3" s="6" t="n">
+        <v>309.6</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>39.19</v>
+      </c>
+      <c r="M3" s="7" t="n">
+        <f aca="false">$K$2/(K3*$F3)</f>
+        <v>0.850775193798449</v>
+      </c>
+      <c r="N3" s="7" t="n">
+        <f aca="false">$L$2/(L3*$F3)</f>
+        <v>0.969507527430467</v>
+      </c>
+      <c r="O3" s="22" t="n">
+        <f aca="false">G3/K3</f>
+        <v>1.17990956072351</v>
+      </c>
+      <c r="P3" s="22" t="n">
+        <f aca="false">H3/L3</f>
+        <v>0.989793314621077</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">C4*C4</f>
+        <v>64000000</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>272.9</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>20.81</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <f aca="false">$G$2/(G4*$F4)</f>
+        <v>0.473525100769513</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <f aca="false">$H$2/(H4*$F4)</f>
+        <v>0.917587698222009</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>174.7</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>20.84</v>
+      </c>
+      <c r="M4" s="7" t="n">
+        <f aca="false">$K$2/(K4*$F4)</f>
+        <v>0.753863766456783</v>
+      </c>
+      <c r="N4" s="7" t="n">
+        <f aca="false">$L$2/(L4*$F4)</f>
+        <v>0.911588291746641</v>
+      </c>
+      <c r="O4" s="22" t="n">
+        <f aca="false">G4/K4</f>
+        <v>1.56210646823125</v>
+      </c>
+      <c r="P4" s="22" t="n">
+        <f aca="false">H4/L4</f>
+        <v>0.998560460652591</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">C5*C5</f>
+        <v>64000000</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>241.7</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>11.35</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <f aca="false">$G$2/(G5*$F5)</f>
+        <v>0.267325196524617</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <f aca="false">$H$2/(H5*$F5)</f>
+        <v>0.841189427312775</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>127.3</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="M5" s="7" t="n">
+        <f aca="false">$K$2/(K5*$F5)</f>
+        <v>0.517282010997643</v>
+      </c>
+      <c r="N5" s="7" t="n">
+        <f aca="false">$L$2/(L5*$F5)</f>
+        <v>0.848102678571429</v>
+      </c>
+      <c r="O5" s="22" t="n">
+        <f aca="false">G5/K5</f>
+        <v>1.89866457187746</v>
+      </c>
+      <c r="P5" s="22" t="n">
+        <f aca="false">H5/L5</f>
+        <v>1.01339285714286</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">C6*C6</f>
+        <v>64000000</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>234.5</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>9.371</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <f aca="false">$G$2/(G6*$F6)</f>
+        <v>0.220426439232409</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <f aca="false">$H$2/(H6*$F6)</f>
+        <v>0.815067762245224</v>
+      </c>
+      <c r="K6" s="6" t="n">
+        <v>120.4</v>
+      </c>
+      <c r="L6" s="6" t="n">
+        <v>9.613</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <f aca="false">$K$2/(K6*$F6)</f>
+        <v>0.437541528239203</v>
+      </c>
+      <c r="N6" s="7" t="n">
+        <f aca="false">$L$2/(L6*$F6)</f>
+        <v>0.790492042026423</v>
+      </c>
+      <c r="O6" s="22" t="n">
+        <f aca="false">G6/K6</f>
+        <v>1.94767441860465</v>
+      </c>
+      <c r="P6" s="22" t="n">
+        <f aca="false">H6/L6</f>
+        <v>0.974825756787683</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">C7*C7</f>
+        <v>64000000</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>233.8</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>6.34</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <f aca="false">$G$2/(G7*$F7)</f>
+        <v>0.138178999144568</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <f aca="false">$H$2/(H7*$F7)</f>
+        <v>0.752957413249211</v>
+      </c>
+      <c r="K7" s="6" t="n">
+        <v>111.6</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>6.094</v>
+      </c>
+      <c r="M7" s="7" t="n">
+        <f aca="false">$K$2/(K7*$F7)</f>
+        <v>0.29502688172043</v>
+      </c>
+      <c r="N7" s="7" t="n">
+        <f aca="false">$L$2/(L7*$F7)</f>
+        <v>0.779352641942895</v>
+      </c>
+      <c r="O7" s="22" t="n">
+        <f aca="false">G7/K7</f>
+        <v>2.09498207885305</v>
+      </c>
+      <c r="P7" s="22" t="n">
+        <f aca="false">H7/L7</f>
+        <v>1.0403675746636</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">C8*C8</f>
+        <v>64000000</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>237.3</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>5.912</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <f aca="false">$G$2/(G8*$F8)</f>
+        <v>0.108912768647282</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <f aca="false">$H$2/(H8*$F8)</f>
+        <v>0.645974289580514</v>
+      </c>
+      <c r="K8" s="6" t="n">
+        <v>111.5</v>
+      </c>
+      <c r="L8" s="6" t="n">
+        <v>5.383</v>
+      </c>
+      <c r="M8" s="7" t="n">
+        <f aca="false">$K$2/(K8*$F8)</f>
+        <v>0.236233183856502</v>
+      </c>
+      <c r="N8" s="7" t="n">
+        <f aca="false">$L$2/(L8*$F8)</f>
+        <v>0.705833178524986</v>
+      </c>
+      <c r="O8" s="22" t="n">
+        <f aca="false">G8/K8</f>
+        <v>2.12825112107623</v>
+      </c>
+      <c r="P8" s="22" t="n">
+        <f aca="false">H8/L8</f>
+        <v>1.09827233884451</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more perfomance results
</commit_message>
<xml_diff>
--- a/Math/Lapack/SVD/svd_benchmarks.xlsx
+++ b/Math/Lapack/SVD/svd_benchmarks.xlsx
@@ -5,20 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="749" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="749" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="scaling" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="effect_dplace" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="scalapack" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="python" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="haswell" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="40">
   <si>
     <t>cluster</t>
   </si>
@@ -126,6 +127,18 @@
   </si>
   <si>
     <t>gcc</t>
+  </si>
+  <si>
+    <t>processor</t>
+  </si>
+  <si>
+    <t>haswell</t>
+  </si>
+  <si>
+    <t>ivybridge</t>
+  </si>
+  <si>
+    <t>Note: could be toolchain atrefact, check!</t>
   </si>
 </sst>
 </file>
@@ -391,7 +404,7 @@
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="600" topLeftCell="A28" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
+      <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4680,7 +4693,7 @@
   </sheetPr>
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -5841,4 +5854,699 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">C2*C2</f>
+        <v>256000000</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>41.44</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>3627</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>359.3</v>
+      </c>
+      <c r="J2" s="7" t="n">
+        <f aca="false">$H$2/(H2*$F2)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="7" t="n">
+        <f aca="false">$I$2/(I2*$F2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">C3*C3</f>
+        <v>256000000</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1938</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>179.2</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <f aca="false">$H$2/(H3*$F3)</f>
+        <v>0.935758513931889</v>
+      </c>
+      <c r="K3" s="7" t="n">
+        <f aca="false">$I$2/(I3*$F3)</f>
+        <v>1.00251116071429</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">C4*C4</f>
+        <v>256000000</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>39.78</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1072</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>91.51</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <f aca="false">$H$2/(H4*$F4)</f>
+        <v>0.845848880597015</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <f aca="false">$I$2/(I4*$F4)</f>
+        <v>0.981586711834772</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">C5*C5</f>
+        <v>256000000</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>39.84</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>747.5</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>49.99</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <f aca="false">$H$2/(H5*$F5)</f>
+        <v>0.606521739130435</v>
+      </c>
+      <c r="K5" s="7" t="n">
+        <f aca="false">$I$2/(I5*$F5)</f>
+        <v>0.898429685937187</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">C6*C6</f>
+        <v>256000000</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>41.43</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>694.7</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>40.73</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <f aca="false">$H$2/(H6*$F6)</f>
+        <v>0.522095868720311</v>
+      </c>
+      <c r="K6" s="7" t="n">
+        <f aca="false">$I$2/(I6*$F6)</f>
+        <v>0.882150748833783</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">C7*C7</f>
+        <v>256000000</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>41.3</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>670.7</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>33.67</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <f aca="false">$H$2/(H7*$F7)</f>
+        <v>0.450648576114507</v>
+      </c>
+      <c r="K7" s="7" t="n">
+        <f aca="false">$I$2/(I7*$F7)</f>
+        <v>0.889268389268389</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">C8*C8</f>
+        <v>256000000</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>39.79</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>634.1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <f aca="false">$H$2/(H8*$F8)</f>
+        <v>0.357494874625453</v>
+      </c>
+      <c r="K8" s="7" t="n">
+        <f aca="false">$I$2/(I8*$F8)</f>
+        <v>0.837919776119403</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">C9*C9</f>
+        <v>256000000</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>39.32</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>632.9</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>23.94</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <f aca="false">$H$2/(H9*$F9)</f>
+        <v>0.286538157686838</v>
+      </c>
+      <c r="K9" s="7" t="n">
+        <f aca="false">$I$2/(I9*$F9)</f>
+        <v>0.750417710944027</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">C10*C10</f>
+        <v>256000000</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>39.7</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>628.6</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>21.73</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <f aca="false">$H$2/(H10*$F10)</f>
+        <v>0.240415208399618</v>
+      </c>
+      <c r="K10" s="7" t="n">
+        <f aca="false">$I$2/(I10*$F10)</f>
+        <v>0.688947691363706</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <f aca="false">16000*16000</f>
+        <v>256000000</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>39.86</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <v>4475</v>
+      </c>
+      <c r="I11" s="6" t="n">
+        <v>605.3</v>
+      </c>
+      <c r="J11" s="7" t="n">
+        <f aca="false">$H$11/(H11*$F11)</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="7" t="n">
+        <f aca="false">$I$11/(I11*$F11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <f aca="false">16000*16000</f>
+        <v>256000000</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>38.86</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <v>2640</v>
+      </c>
+      <c r="I12" s="6" t="n">
+        <v>306.3</v>
+      </c>
+      <c r="J12" s="7" t="n">
+        <f aca="false">$H$11/(H12*$F12)</f>
+        <v>0.847537878787879</v>
+      </c>
+      <c r="K12" s="7" t="n">
+        <f aca="false">$I$11/(I12*$F12)</f>
+        <v>0.988083578191316</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <f aca="false">16000*16000</f>
+        <v>256000000</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>36.48</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <v>1450</v>
+      </c>
+      <c r="I13" s="6" t="n">
+        <v>158.3</v>
+      </c>
+      <c r="J13" s="7" t="n">
+        <f aca="false">$H$11/(H13*$F13)</f>
+        <v>0.771551724137931</v>
+      </c>
+      <c r="K13" s="7" t="n">
+        <f aca="false">$I$11/(I13*$F13)</f>
+        <v>0.955938092229943</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <f aca="false">16000*16000</f>
+        <v>256000000</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>38.65</v>
+      </c>
+      <c r="H14" s="6" t="n">
+        <v>1012</v>
+      </c>
+      <c r="I14" s="6" t="n">
+        <v>84.39</v>
+      </c>
+      <c r="J14" s="7" t="n">
+        <f aca="false">$H$11/(H14*$F14)</f>
+        <v>0.55274209486166</v>
+      </c>
+      <c r="K14" s="7" t="n">
+        <f aca="false">$I$11/(I14*$F14)</f>
+        <v>0.896581348501007</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <f aca="false">16000*16000</f>
+        <v>256000000</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>34.87</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <v>947.1</v>
+      </c>
+      <c r="I15" s="6" t="n">
+        <v>70.43</v>
+      </c>
+      <c r="J15" s="7" t="n">
+        <f aca="false">$H$11/(H15*$F15)</f>
+        <v>0.472494984690107</v>
+      </c>
+      <c r="K15" s="7" t="n">
+        <f aca="false">$I$11/(I15*$F15)</f>
+        <v>0.85943489990061</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <f aca="false">16000*16000</f>
+        <v>256000000</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>36.39</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>874.7</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>45.05</v>
+      </c>
+      <c r="J16" s="7" t="n">
+        <f aca="false">$H$11/(H16*$F16)</f>
+        <v>0.319752486566823</v>
+      </c>
+      <c r="K16" s="7" t="n">
+        <f aca="false">$I$11/(I16*$F16)</f>
+        <v>0.839761376248613</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <f aca="false">16000*16000</f>
+        <v>256000000</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>34.93</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>855.8</v>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>37.14</v>
+      </c>
+      <c r="J17" s="7" t="n">
+        <f aca="false">$H$11/(H17*$F17)</f>
+        <v>0.261451273662071</v>
+      </c>
+      <c r="K17" s="7" t="n">
+        <f aca="false">$I$11/(I17*$F17)</f>
+        <v>0.814889606892838</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H20" s="0" t="n">
+        <f aca="false">H2/H11</f>
+        <v>0.810502793296089</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">I2/I11</f>
+        <v>0.59358995539402</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H21" s="0" t="n">
+        <f aca="false">H10/H17</f>
+        <v>0.734517410609956</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">I10/I17</f>
+        <v>0.585083467959074</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>